<commit_message>
Added 40 more pairs and updated pairs excel file.
</commit_message>
<xml_diff>
--- a/faza1_tabela.xlsx
+++ b/faza1_tabela.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24119"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_8AE502EB0B3D2FD929D5ECC45C0837D65FA74751" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
   </bookViews>
   <sheets>
     <sheet name="bb" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="737">
   <si>
     <t>ProgrammingLanguageName</t>
   </si>
@@ -2042,12 +2041,207 @@
   </si>
   <si>
     <t>Dohvati vrednost i ispis je na standarnom izlazu na konzoli.</t>
+  </si>
+  <si>
+    <t>2_convertIntToString5</t>
+  </si>
+  <si>
+    <t>Uradi obradu konverzije celobrojnog broja u string.</t>
+  </si>
+  <si>
+    <t>2_convertIntToString6</t>
+  </si>
+  <si>
+    <t>Pretvaranje celih brojeva.</t>
+  </si>
+  <si>
+    <t>2_convertIntToString7</t>
+  </si>
+  <si>
+    <t>Pretvaranje brojeva u stringove.</t>
+  </si>
+  <si>
+    <t>2_convertIntToString8</t>
+  </si>
+  <si>
+    <t>Prebaci ceo broj u string.</t>
+  </si>
+  <si>
+    <t>2_convertIntToString9</t>
+  </si>
+  <si>
+    <t>Konvertovanje u string.</t>
+  </si>
+  <si>
+    <t>Fajl za rad sa stringovima. Operacije nad stringovima itd…</t>
+  </si>
+  <si>
+    <t>3_pq1</t>
+  </si>
+  <si>
+    <t>Ubaci u prioritetni red podatke izvucene iz zahteva.</t>
+  </si>
+  <si>
+    <t>3_pq2</t>
+  </si>
+  <si>
+    <t>Uradi obradu zahteva po prioritetima.</t>
+  </si>
+  <si>
+    <t>3_pq3</t>
+  </si>
+  <si>
+    <t>3_pq4</t>
+  </si>
+  <si>
+    <t>3_pq5</t>
+  </si>
+  <si>
+    <t>Varijable izvucene iz klijentskog zahteva ubaciti u prioritetni red.</t>
+  </si>
+  <si>
+    <t>Izbrisati iz prioritetnog reda deset podataka.</t>
+  </si>
+  <si>
+    <t>Obraditi podataka po prioritetima.</t>
+  </si>
+  <si>
+    <t>Fajl sa razlicitim strukturama podataka, Stekovi, redovi itd…</t>
+  </si>
+  <si>
+    <t>4_sud1</t>
+  </si>
+  <si>
+    <t>Konverzija tipova u datum.</t>
+  </si>
+  <si>
+    <t>4_sud2</t>
+  </si>
+  <si>
+    <t>4_sud3</t>
+  </si>
+  <si>
+    <t>4_sud4</t>
+  </si>
+  <si>
+    <t>4_sud5</t>
+  </si>
+  <si>
+    <t>Pretvori stringove primljene kao parametre zahteva u datume.</t>
+  </si>
+  <si>
+    <t>Od niza stringova, formiraj jedan konkatenirani string i probaj da ga pretvoris u datum.</t>
+  </si>
+  <si>
+    <t>Uradi operaciju nad parovima stringova i pretvori rezultat u datum.</t>
+  </si>
+  <si>
+    <t>Podeli string da vise malih delova, i iz tih delova probaj da napravis datum.</t>
+  </si>
+  <si>
+    <t>6_saveListF1</t>
+  </si>
+  <si>
+    <t>Sadrzaj dve liste kombinovane sacuvaj u okviru tekstualnog fajla.</t>
+  </si>
+  <si>
+    <t>6_saveListF2</t>
+  </si>
+  <si>
+    <t>6_saveListF3</t>
+  </si>
+  <si>
+    <t>6_saveListF4</t>
+  </si>
+  <si>
+    <t>6_saveListF5</t>
+  </si>
+  <si>
+    <t>Spoji par listi prosledjenih preko klijenstkoj zahteva i prodaj da ih sacuvas u txt fajlu.</t>
+  </si>
+  <si>
+    <t>Indeksiranu listu sacuvaj u fajlu.</t>
+  </si>
+  <si>
+    <t>Listu interno implementiranu kao jednostruku usnimiti u fajl.</t>
+  </si>
+  <si>
+    <t>Listu interno implementiranu kao dvostruko ulanacanu usnimiti u text fajl.</t>
+  </si>
+  <si>
+    <t>Fajl za rad sa datotekama.</t>
+  </si>
+  <si>
+    <t>8_cm1</t>
+  </si>
+  <si>
+    <t>8_cm2</t>
+  </si>
+  <si>
+    <t>8_cm3</t>
+  </si>
+  <si>
+    <t>8_cm4</t>
+  </si>
+  <si>
+    <t>8_cm5</t>
+  </si>
+  <si>
+    <t>Ubaci u matricu implementiranu kao dvodimenzijalni niz novu vrednost.</t>
+  </si>
+  <si>
+    <t>Iz matrice implementirane preko dvodimenzijalnog niza, uklonoiti element na poziciji 3 3.</t>
+  </si>
+  <si>
+    <t>Iz matrice dohvatiti samo prvi red i ispisati ga na standardnom izlazu.</t>
+  </si>
+  <si>
+    <t>Vratiti elemente koji se nalazi na dijagonali matrice.</t>
+  </si>
+  <si>
+    <t>Pre brisanja matrice zabune ispisi njene elemente.</t>
+  </si>
+  <si>
+    <t>Fajlovi sa razlicitim strukturama podataka.</t>
+  </si>
+  <si>
+    <t>12_aes1</t>
+  </si>
+  <si>
+    <t>Iskoristiti aes enkripciju da bi se zastitili bitni podaci.</t>
+  </si>
+  <si>
+    <t>12_aes2</t>
+  </si>
+  <si>
+    <t>12_aes3</t>
+  </si>
+  <si>
+    <t>12_aes4</t>
+  </si>
+  <si>
+    <t>12_aes5</t>
+  </si>
+  <si>
+    <t>Aes enkripcija promenljivih iz dokument menadzera.</t>
+  </si>
+  <si>
+    <t>Enkriptovanje sifre sa aes algoritmom.</t>
+  </si>
+  <si>
+    <t>Fajlovi za enkripciju sifre.</t>
+  </si>
+  <si>
+    <t>Dekripcija dva ulazna parametra preko aes algoritma.</t>
+  </si>
+  <si>
+    <t>Sifrovanje osetljivih podataka raznim algoritmima za enkripciju.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -2629,7 +2823,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2661,27 +2855,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2713,24 +2889,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2906,20 +3064,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E350"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B350"/>
+    <sheetView tabSelected="1" topLeftCell="D325" workbookViewId="0">
+      <selection activeCell="E351" sqref="E351"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="84.28515625" customWidth="1"/>
-    <col min="3" max="3" width="73.5703125" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" customWidth="1"/>
-    <col min="5" max="5" width="144.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
+    <col min="2" max="2" width="84.33203125" customWidth="1"/>
+    <col min="3" max="3" width="73.5546875" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" customWidth="1"/>
+    <col min="5" max="5" width="144.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -8362,244 +8520,514 @@
         <v>671</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
+    <row r="321" spans="1:5">
       <c r="A321" t="s">
         <v>5</v>
       </c>
       <c r="B321" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="322" spans="1:2">
+      <c r="C321" t="s">
+        <v>682</v>
+      </c>
+      <c r="D321" t="s">
+        <v>672</v>
+      </c>
+      <c r="E321" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5">
       <c r="A322" t="s">
         <v>5</v>
       </c>
       <c r="B322" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="323" spans="1:2">
+      <c r="C322" t="s">
+        <v>682</v>
+      </c>
+      <c r="D322" t="s">
+        <v>674</v>
+      </c>
+      <c r="E322" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5">
       <c r="A323" t="s">
         <v>5</v>
       </c>
       <c r="B323" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="324" spans="1:2">
+      <c r="C323" t="s">
+        <v>682</v>
+      </c>
+      <c r="D323" t="s">
+        <v>676</v>
+      </c>
+      <c r="E323" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5">
       <c r="A324" t="s">
         <v>5</v>
       </c>
       <c r="B324" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="325" spans="1:2">
+      <c r="C324" t="s">
+        <v>682</v>
+      </c>
+      <c r="D324" t="s">
+        <v>678</v>
+      </c>
+      <c r="E324" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5">
       <c r="A325" t="s">
         <v>5</v>
       </c>
       <c r="B325" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="326" spans="1:2">
+      <c r="C325" t="s">
+        <v>682</v>
+      </c>
+      <c r="D325" t="s">
+        <v>680</v>
+      </c>
+      <c r="E325" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5">
       <c r="A326" t="s">
         <v>5</v>
       </c>
       <c r="B326" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="327" spans="1:2">
+      <c r="C326" t="s">
+        <v>693</v>
+      </c>
+      <c r="D326" t="s">
+        <v>683</v>
+      </c>
+      <c r="E326" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5">
       <c r="A327" t="s">
         <v>5</v>
       </c>
       <c r="B327" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="328" spans="1:2">
+      <c r="C327" t="s">
+        <v>693</v>
+      </c>
+      <c r="D327" t="s">
+        <v>685</v>
+      </c>
+      <c r="E327" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5">
       <c r="A328" t="s">
         <v>5</v>
       </c>
       <c r="B328" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="329" spans="1:2">
+      <c r="C328" t="s">
+        <v>693</v>
+      </c>
+      <c r="D328" t="s">
+        <v>687</v>
+      </c>
+      <c r="E328" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5">
       <c r="A329" t="s">
         <v>5</v>
       </c>
       <c r="B329" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="330" spans="1:2">
+      <c r="C329" t="s">
+        <v>693</v>
+      </c>
+      <c r="D329" t="s">
+        <v>688</v>
+      </c>
+      <c r="E329" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5">
       <c r="A330" t="s">
         <v>5</v>
       </c>
       <c r="B330" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="331" spans="1:2">
+      <c r="C330" t="s">
+        <v>693</v>
+      </c>
+      <c r="D330" t="s">
+        <v>689</v>
+      </c>
+      <c r="E330" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5">
       <c r="A331" t="s">
         <v>5</v>
       </c>
       <c r="B331" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="332" spans="1:2">
+      <c r="C331" t="s">
+        <v>531</v>
+      </c>
+      <c r="D331" t="s">
+        <v>694</v>
+      </c>
+      <c r="E331" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5">
       <c r="A332" t="s">
         <v>5</v>
       </c>
       <c r="B332" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="333" spans="1:2">
+      <c r="C332" t="s">
+        <v>531</v>
+      </c>
+      <c r="D332" t="s">
+        <v>696</v>
+      </c>
+      <c r="E332" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5">
       <c r="A333" t="s">
         <v>5</v>
       </c>
       <c r="B333" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="334" spans="1:2">
+      <c r="C333" t="s">
+        <v>531</v>
+      </c>
+      <c r="D333" t="s">
+        <v>697</v>
+      </c>
+      <c r="E333" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5">
       <c r="A334" t="s">
         <v>5</v>
       </c>
       <c r="B334" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="335" spans="1:2">
+      <c r="C334" t="s">
+        <v>531</v>
+      </c>
+      <c r="D334" t="s">
+        <v>698</v>
+      </c>
+      <c r="E334" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5">
       <c r="A335" t="s">
         <v>5</v>
       </c>
       <c r="B335" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="336" spans="1:2">
+      <c r="C335" t="s">
+        <v>531</v>
+      </c>
+      <c r="D335" t="s">
+        <v>699</v>
+      </c>
+      <c r="E335" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5">
       <c r="A336" t="s">
         <v>5</v>
       </c>
       <c r="B336" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="337" spans="1:2">
+      <c r="C336" t="s">
+        <v>714</v>
+      </c>
+      <c r="D336" t="s">
+        <v>704</v>
+      </c>
+      <c r="E336" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5">
       <c r="A337" t="s">
         <v>5</v>
       </c>
       <c r="B337" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="338" spans="1:2">
+      <c r="C337" t="s">
+        <v>714</v>
+      </c>
+      <c r="D337" t="s">
+        <v>706</v>
+      </c>
+      <c r="E337" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5">
       <c r="A338" t="s">
         <v>5</v>
       </c>
       <c r="B338" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="339" spans="1:2">
+      <c r="C338" t="s">
+        <v>714</v>
+      </c>
+      <c r="D338" t="s">
+        <v>707</v>
+      </c>
+      <c r="E338" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5">
       <c r="A339" t="s">
         <v>5</v>
       </c>
       <c r="B339" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="340" spans="1:2">
+      <c r="C339" t="s">
+        <v>714</v>
+      </c>
+      <c r="D339" t="s">
+        <v>708</v>
+      </c>
+      <c r="E339" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5">
       <c r="A340" t="s">
         <v>5</v>
       </c>
       <c r="B340" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="341" spans="1:2">
+      <c r="C340" t="s">
+        <v>714</v>
+      </c>
+      <c r="D340" t="s">
+        <v>709</v>
+      </c>
+      <c r="E340" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5">
       <c r="A341" t="s">
         <v>5</v>
       </c>
       <c r="B341" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="342" spans="1:2">
+      <c r="C341" t="s">
+        <v>725</v>
+      </c>
+      <c r="D341" t="s">
+        <v>715</v>
+      </c>
+      <c r="E341" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5">
       <c r="A342" t="s">
         <v>5</v>
       </c>
       <c r="B342" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="343" spans="1:2">
+      <c r="C342" t="s">
+        <v>725</v>
+      </c>
+      <c r="D342" t="s">
+        <v>716</v>
+      </c>
+      <c r="E342" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5">
       <c r="A343" t="s">
         <v>5</v>
       </c>
       <c r="B343" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="344" spans="1:2">
+      <c r="C343" t="s">
+        <v>725</v>
+      </c>
+      <c r="D343" t="s">
+        <v>717</v>
+      </c>
+      <c r="E343" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5">
       <c r="A344" t="s">
         <v>5</v>
       </c>
       <c r="B344" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="345" spans="1:2">
+      <c r="C344" t="s">
+        <v>725</v>
+      </c>
+      <c r="D344" t="s">
+        <v>718</v>
+      </c>
+      <c r="E344" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5">
       <c r="A345" t="s">
         <v>5</v>
       </c>
       <c r="B345" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="346" spans="1:2">
+      <c r="C345" t="s">
+        <v>725</v>
+      </c>
+      <c r="D345" t="s">
+        <v>719</v>
+      </c>
+      <c r="E345" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5">
       <c r="A346" t="s">
         <v>5</v>
       </c>
       <c r="B346" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="347" spans="1:2">
+      <c r="C346" t="s">
+        <v>734</v>
+      </c>
+      <c r="D346" t="s">
+        <v>726</v>
+      </c>
+      <c r="E346" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5">
       <c r="A347" t="s">
         <v>5</v>
       </c>
       <c r="B347" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="348" spans="1:2">
+      <c r="C347" t="s">
+        <v>734</v>
+      </c>
+      <c r="D347" t="s">
+        <v>728</v>
+      </c>
+      <c r="E347" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5">
       <c r="A348" t="s">
         <v>5</v>
       </c>
       <c r="B348" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="349" spans="1:2">
+      <c r="C348" t="s">
+        <v>734</v>
+      </c>
+      <c r="D348" t="s">
+        <v>729</v>
+      </c>
+      <c r="E348" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5">
       <c r="A349" t="s">
         <v>5</v>
       </c>
       <c r="B349" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="350" spans="1:2">
+      <c r="C349" t="s">
+        <v>734</v>
+      </c>
+      <c r="D349" t="s">
+        <v>730</v>
+      </c>
+      <c r="E349" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5">
       <c r="A350" t="s">
         <v>5</v>
       </c>
       <c r="B350" t="s">
         <v>6</v>
+      </c>
+      <c r="C350" t="s">
+        <v>734</v>
+      </c>
+      <c r="D350" t="s">
+        <v>731</v>
+      </c>
+      <c r="E350" t="s">
+        <v>736</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added last 7 files and updated faza1_table.xlsx
</commit_message>
<xml_diff>
--- a/faza1_tabela.xlsx
+++ b/faza1_tabela.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jokan\Documents\LENA\Masters\OPJ\natural-language-processing-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E125EA5D-C54A-4DDF-95FB-0AC451BC7AC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0DB17E-8B59-490C-89DA-D432E0A4CB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-98" windowWidth="28995" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2733" uniqueCount="1151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2750" uniqueCount="1165">
   <si>
     <t>ProgrammingLanguageName</t>
   </si>
@@ -3473,6 +3473,48 @@
   </si>
   <si>
     <t>Parsiranje csv fajla u posebnu klasu</t>
+  </si>
+  <si>
+    <t>Nadovezivanje fajlova tako da se cuva samo zaglavlje prvog fajla a ostala zaglavlja se uklanjanju</t>
+  </si>
+  <si>
+    <t>96_mergeFileKeepFirstHeaderOnly</t>
+  </si>
+  <si>
+    <t>95_findAverageSalary</t>
+  </si>
+  <si>
+    <t>95_findAverageValueAcrossTable</t>
+  </si>
+  <si>
+    <t>Pronalazenje srednje vrednosti iz svih celija tabele</t>
+  </si>
+  <si>
+    <t>Pronalazenje srednje vrednosti kolone za platu</t>
+  </si>
+  <si>
+    <t>92_getFirstAndLastSentenceFile</t>
+  </si>
+  <si>
+    <t>92_getMostCommonWordFromFile</t>
+  </si>
+  <si>
+    <t>Ekstrakcija najcesce koriscene reci u tekstualnom fajlu</t>
+  </si>
+  <si>
+    <t>Ekstrakcija prve i poslednje recenice iz tekstualnog fajla</t>
+  </si>
+  <si>
+    <t>79_copyFile1</t>
+  </si>
+  <si>
+    <t>79_copyFile2</t>
+  </si>
+  <si>
+    <t>Kopiranje fajla u vise razlicitih lokacija datim u nizu</t>
+  </si>
+  <si>
+    <t>Kopiranje fajla n puta u odredjenu putanju</t>
   </si>
 </sst>
 </file>
@@ -4338,10 +4380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E552"/>
+  <dimension ref="A1:E550"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C509" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E543" sqref="E543"/>
+    <sheetView tabSelected="1" topLeftCell="C401" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E409" sqref="E409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11283,10 +11325,10 @@
         <v>848</v>
       </c>
       <c r="D408" t="s">
-        <v>861</v>
+        <v>1161</v>
       </c>
       <c r="E408" t="s">
-        <v>862</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.3">
@@ -11297,13 +11339,13 @@
         <v>6</v>
       </c>
       <c r="C409" t="s">
-        <v>863</v>
+        <v>848</v>
       </c>
       <c r="D409" t="s">
-        <v>864</v>
+        <v>1162</v>
       </c>
       <c r="E409" t="s">
-        <v>871</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.3">
@@ -11314,13 +11356,13 @@
         <v>6</v>
       </c>
       <c r="C410" t="s">
-        <v>863</v>
+        <v>848</v>
       </c>
       <c r="D410" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="E410" t="s">
-        <v>872</v>
+        <v>862</v>
       </c>
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.3">
@@ -11334,10 +11376,10 @@
         <v>863</v>
       </c>
       <c r="D411" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="E411" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.3">
@@ -11351,10 +11393,10 @@
         <v>863</v>
       </c>
       <c r="D412" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="E412" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.3">
@@ -11368,10 +11410,10 @@
         <v>863</v>
       </c>
       <c r="D413" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="E413" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.3">
@@ -11385,10 +11427,10 @@
         <v>863</v>
       </c>
       <c r="D414" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="E414" t="s">
-        <v>776</v>
+        <v>874</v>
       </c>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.3">
@@ -11402,10 +11444,10 @@
         <v>863</v>
       </c>
       <c r="D415" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="E415" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.3">
@@ -11416,13 +11458,13 @@
         <v>6</v>
       </c>
       <c r="C416" t="s">
-        <v>877</v>
+        <v>863</v>
       </c>
       <c r="D416" t="s">
-        <v>884</v>
+        <v>869</v>
       </c>
       <c r="E416" t="s">
-        <v>883</v>
+        <v>776</v>
       </c>
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.3">
@@ -11433,13 +11475,13 @@
         <v>6</v>
       </c>
       <c r="C417" t="s">
-        <v>877</v>
+        <v>863</v>
       </c>
       <c r="D417" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="E417" t="s">
-        <v>886</v>
+        <v>876</v>
       </c>
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.3">
@@ -11453,10 +11495,10 @@
         <v>877</v>
       </c>
       <c r="D418" t="s">
-        <v>879</v>
+        <v>884</v>
       </c>
       <c r="E418" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.3">
@@ -11470,10 +11512,10 @@
         <v>877</v>
       </c>
       <c r="D419" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E419" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.3">
@@ -11487,10 +11529,10 @@
         <v>877</v>
       </c>
       <c r="D420" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="E420" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.3">
@@ -11504,10 +11546,10 @@
         <v>877</v>
       </c>
       <c r="D421" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="E421" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.3">
@@ -11521,10 +11563,10 @@
         <v>877</v>
       </c>
       <c r="D422" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="E422" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.3">
@@ -11535,13 +11577,13 @@
         <v>6</v>
       </c>
       <c r="C423" t="s">
-        <v>892</v>
+        <v>877</v>
       </c>
       <c r="D423" t="s">
-        <v>893</v>
+        <v>882</v>
       </c>
       <c r="E423" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.3">
@@ -11552,13 +11594,13 @@
         <v>6</v>
       </c>
       <c r="C424" t="s">
-        <v>892</v>
+        <v>877</v>
       </c>
       <c r="D424" t="s">
-        <v>895</v>
+        <v>885</v>
       </c>
       <c r="E424" t="s">
-        <v>899</v>
+        <v>888</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.3">
@@ -11572,10 +11614,10 @@
         <v>892</v>
       </c>
       <c r="D425" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="E425" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.3">
@@ -11589,10 +11631,10 @@
         <v>892</v>
       </c>
       <c r="D426" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="E426" t="s">
-        <v>894</v>
+        <v>899</v>
       </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.3">
@@ -11606,10 +11648,10 @@
         <v>892</v>
       </c>
       <c r="D427" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="E427" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.3">
@@ -11620,13 +11662,13 @@
         <v>6</v>
       </c>
       <c r="C428" t="s">
-        <v>902</v>
+        <v>892</v>
       </c>
       <c r="D428" t="s">
-        <v>903</v>
+        <v>898</v>
       </c>
       <c r="E428" t="s">
-        <v>904</v>
+        <v>894</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.3">
@@ -11637,13 +11679,13 @@
         <v>6</v>
       </c>
       <c r="C429" t="s">
-        <v>902</v>
+        <v>892</v>
       </c>
       <c r="D429" t="s">
-        <v>905</v>
+        <v>900</v>
       </c>
       <c r="E429" t="s">
-        <v>906</v>
+        <v>901</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.3">
@@ -11657,10 +11699,10 @@
         <v>902</v>
       </c>
       <c r="D430" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="E430" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.3">
@@ -11674,10 +11716,10 @@
         <v>902</v>
       </c>
       <c r="D431" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="E431" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.3">
@@ -11691,10 +11733,10 @@
         <v>902</v>
       </c>
       <c r="D432" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="E432" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.3">
@@ -11705,13 +11747,13 @@
         <v>6</v>
       </c>
       <c r="C433" t="s">
-        <v>913</v>
+        <v>902</v>
       </c>
       <c r="D433" t="s">
-        <v>914</v>
+        <v>909</v>
       </c>
       <c r="E433" t="s">
-        <v>920</v>
+        <v>910</v>
       </c>
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.3">
@@ -11722,13 +11764,13 @@
         <v>6</v>
       </c>
       <c r="C434" t="s">
-        <v>913</v>
+        <v>902</v>
       </c>
       <c r="D434" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="E434" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.3">
@@ -11742,10 +11784,10 @@
         <v>913</v>
       </c>
       <c r="D435" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="E435" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.3">
@@ -11759,10 +11801,10 @@
         <v>913</v>
       </c>
       <c r="D436" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="E436" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.3">
@@ -11776,10 +11818,10 @@
         <v>913</v>
       </c>
       <c r="D437" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="E437" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.3">
@@ -11793,10 +11835,10 @@
         <v>913</v>
       </c>
       <c r="D438" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="E438" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.3">
@@ -11807,13 +11849,13 @@
         <v>6</v>
       </c>
       <c r="C439" t="s">
-        <v>926</v>
+        <v>913</v>
       </c>
       <c r="D439" t="s">
-        <v>927</v>
+        <v>918</v>
       </c>
       <c r="E439" t="s">
-        <v>934</v>
+        <v>924</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.3">
@@ -11824,13 +11866,13 @@
         <v>6</v>
       </c>
       <c r="C440" t="s">
-        <v>926</v>
+        <v>913</v>
       </c>
       <c r="D440" t="s">
-        <v>928</v>
+        <v>919</v>
       </c>
       <c r="E440" t="s">
-        <v>935</v>
+        <v>925</v>
       </c>
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.3">
@@ -11844,10 +11886,10 @@
         <v>926</v>
       </c>
       <c r="D441" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="E441" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.3">
@@ -11861,10 +11903,10 @@
         <v>926</v>
       </c>
       <c r="D442" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="E442" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.3">
@@ -11878,10 +11920,10 @@
         <v>926</v>
       </c>
       <c r="D443" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="E443" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.3">
@@ -11895,10 +11937,10 @@
         <v>926</v>
       </c>
       <c r="D444" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="E444" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.3">
@@ -11912,10 +11954,10 @@
         <v>926</v>
       </c>
       <c r="D445" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="E445" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.3">
@@ -11926,13 +11968,13 @@
         <v>6</v>
       </c>
       <c r="C446" t="s">
-        <v>941</v>
+        <v>926</v>
       </c>
       <c r="D446" t="s">
-        <v>942</v>
+        <v>932</v>
       </c>
       <c r="E446" t="s">
-        <v>955</v>
+        <v>939</v>
       </c>
     </row>
     <row r="447" spans="1:5" x14ac:dyDescent="0.3">
@@ -11943,13 +11985,13 @@
         <v>6</v>
       </c>
       <c r="C447" t="s">
-        <v>941</v>
+        <v>926</v>
       </c>
       <c r="D447" t="s">
-        <v>943</v>
+        <v>933</v>
       </c>
       <c r="E447" t="s">
-        <v>949</v>
+        <v>940</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.3">
@@ -11963,10 +12005,10 @@
         <v>941</v>
       </c>
       <c r="D448" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="E448" t="s">
-        <v>950</v>
+        <v>955</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.3">
@@ -11980,10 +12022,10 @@
         <v>941</v>
       </c>
       <c r="D449" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="E449" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.3">
@@ -11997,10 +12039,10 @@
         <v>941</v>
       </c>
       <c r="D450" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="E450" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.3">
@@ -12014,10 +12056,10 @@
         <v>941</v>
       </c>
       <c r="D451" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="E451" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.3">
@@ -12031,10 +12073,10 @@
         <v>941</v>
       </c>
       <c r="D452" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E452" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.3">
@@ -12045,13 +12087,13 @@
         <v>6</v>
       </c>
       <c r="C453" t="s">
-        <v>956</v>
+        <v>941</v>
       </c>
       <c r="D453" t="s">
-        <v>957</v>
+        <v>947</v>
       </c>
       <c r="E453" t="s">
-        <v>964</v>
+        <v>953</v>
       </c>
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.3">
@@ -12062,13 +12104,13 @@
         <v>6</v>
       </c>
       <c r="C454" t="s">
-        <v>956</v>
+        <v>941</v>
       </c>
       <c r="D454" t="s">
-        <v>958</v>
+        <v>948</v>
       </c>
       <c r="E454" t="s">
-        <v>965</v>
+        <v>954</v>
       </c>
     </row>
     <row r="455" spans="1:5" x14ac:dyDescent="0.3">
@@ -12082,10 +12124,10 @@
         <v>956</v>
       </c>
       <c r="D455" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E455" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="456" spans="1:5" x14ac:dyDescent="0.3">
@@ -12099,10 +12141,10 @@
         <v>956</v>
       </c>
       <c r="D456" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="E456" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.3">
@@ -12116,10 +12158,10 @@
         <v>956</v>
       </c>
       <c r="D457" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="E457" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.3">
@@ -12133,10 +12175,10 @@
         <v>956</v>
       </c>
       <c r="D458" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="E458" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.3">
@@ -12150,10 +12192,10 @@
         <v>956</v>
       </c>
       <c r="D459" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="E459" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.3">
@@ -12164,13 +12206,13 @@
         <v>6</v>
       </c>
       <c r="C460" t="s">
-        <v>971</v>
+        <v>956</v>
       </c>
       <c r="D460" t="s">
-        <v>972</v>
+        <v>962</v>
       </c>
       <c r="E460" t="s">
-        <v>979</v>
+        <v>969</v>
       </c>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.3">
@@ -12181,13 +12223,13 @@
         <v>6</v>
       </c>
       <c r="C461" t="s">
-        <v>971</v>
+        <v>956</v>
       </c>
       <c r="D461" t="s">
-        <v>973</v>
+        <v>963</v>
       </c>
       <c r="E461" t="s">
-        <v>980</v>
+        <v>970</v>
       </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.3">
@@ -12201,10 +12243,10 @@
         <v>971</v>
       </c>
       <c r="D462" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="E462" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.3">
@@ -12218,10 +12260,10 @@
         <v>971</v>
       </c>
       <c r="D463" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="E463" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.3">
@@ -12235,10 +12277,10 @@
         <v>971</v>
       </c>
       <c r="D464" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="E464" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="465" spans="1:5" x14ac:dyDescent="0.3">
@@ -12252,10 +12294,10 @@
         <v>971</v>
       </c>
       <c r="D465" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="E465" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.3">
@@ -12269,10 +12311,10 @@
         <v>971</v>
       </c>
       <c r="D466" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="E466" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="467" spans="1:5" x14ac:dyDescent="0.3">
@@ -12283,13 +12325,13 @@
         <v>6</v>
       </c>
       <c r="C467" t="s">
-        <v>986</v>
+        <v>971</v>
       </c>
       <c r="D467" t="s">
-        <v>987</v>
+        <v>977</v>
       </c>
       <c r="E467" t="s">
-        <v>993</v>
+        <v>984</v>
       </c>
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.3">
@@ -12300,13 +12342,13 @@
         <v>6</v>
       </c>
       <c r="C468" t="s">
-        <v>986</v>
+        <v>971</v>
       </c>
       <c r="D468" t="s">
-        <v>988</v>
+        <v>978</v>
       </c>
       <c r="E468" t="s">
-        <v>994</v>
+        <v>985</v>
       </c>
     </row>
     <row r="469" spans="1:5" x14ac:dyDescent="0.3">
@@ -12320,10 +12362,10 @@
         <v>986</v>
       </c>
       <c r="D469" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="E469" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.3">
@@ -12337,10 +12379,10 @@
         <v>986</v>
       </c>
       <c r="D470" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="E470" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.3">
@@ -12354,10 +12396,10 @@
         <v>986</v>
       </c>
       <c r="D471" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="E471" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="472" spans="1:5" x14ac:dyDescent="0.3">
@@ -12371,10 +12413,10 @@
         <v>986</v>
       </c>
       <c r="D472" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E472" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.3">
@@ -12385,13 +12427,13 @@
         <v>6</v>
       </c>
       <c r="C473" t="s">
-        <v>999</v>
+        <v>986</v>
       </c>
       <c r="D473" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
       <c r="E473" t="s">
-        <v>1006</v>
+        <v>997</v>
       </c>
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.3">
@@ -12402,13 +12444,13 @@
         <v>6</v>
       </c>
       <c r="C474" t="s">
-        <v>999</v>
+        <v>986</v>
       </c>
       <c r="D474" t="s">
-        <v>1001</v>
+        <v>992</v>
       </c>
       <c r="E474" t="s">
-        <v>1007</v>
+        <v>998</v>
       </c>
     </row>
     <row r="475" spans="1:5" x14ac:dyDescent="0.3">
@@ -12422,10 +12464,10 @@
         <v>999</v>
       </c>
       <c r="D475" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="E475" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.3">
@@ -12439,10 +12481,10 @@
         <v>999</v>
       </c>
       <c r="D476" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E476" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.3">
@@ -12456,10 +12498,10 @@
         <v>999</v>
       </c>
       <c r="D477" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="E477" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.3">
@@ -12473,10 +12515,10 @@
         <v>999</v>
       </c>
       <c r="D478" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="E478" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.3">
@@ -12487,13 +12529,13 @@
         <v>6</v>
       </c>
       <c r="C479" t="s">
-        <v>1012</v>
+        <v>999</v>
       </c>
       <c r="D479" t="s">
-        <v>1013</v>
+        <v>1004</v>
       </c>
       <c r="E479" t="s">
-        <v>1019</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.3">
@@ -12504,13 +12546,13 @@
         <v>6</v>
       </c>
       <c r="C480" t="s">
-        <v>1012</v>
+        <v>999</v>
       </c>
       <c r="D480" t="s">
-        <v>1014</v>
+        <v>1005</v>
       </c>
       <c r="E480" t="s">
-        <v>1020</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="481" spans="1:5" x14ac:dyDescent="0.3">
@@ -12524,10 +12566,10 @@
         <v>1012</v>
       </c>
       <c r="D481" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="E481" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="482" spans="1:5" x14ac:dyDescent="0.3">
@@ -12541,10 +12583,10 @@
         <v>1012</v>
       </c>
       <c r="D482" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="E482" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.3">
@@ -12558,10 +12600,10 @@
         <v>1012</v>
       </c>
       <c r="D483" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="E483" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.3">
@@ -12575,10 +12617,10 @@
         <v>1012</v>
       </c>
       <c r="D484" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="E484" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.3">
@@ -12589,13 +12631,13 @@
         <v>6</v>
       </c>
       <c r="C485" t="s">
-        <v>1025</v>
+        <v>1012</v>
       </c>
       <c r="D485" t="s">
-        <v>1026</v>
+        <v>1017</v>
       </c>
       <c r="E485" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.3">
@@ -12606,13 +12648,13 @@
         <v>6</v>
       </c>
       <c r="C486" t="s">
-        <v>1025</v>
+        <v>1012</v>
       </c>
       <c r="D486" t="s">
-        <v>1028</v>
+        <v>1018</v>
       </c>
       <c r="E486" t="s">
-        <v>1029</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.3">
@@ -12626,10 +12668,10 @@
         <v>1025</v>
       </c>
       <c r="D487" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="E487" t="s">
-        <v>1034</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.3">
@@ -12643,10 +12685,10 @@
         <v>1025</v>
       </c>
       <c r="D488" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="E488" t="s">
-        <v>1035</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="489" spans="1:5" x14ac:dyDescent="0.3">
@@ -12660,10 +12702,10 @@
         <v>1025</v>
       </c>
       <c r="D489" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="E489" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="490" spans="1:5" x14ac:dyDescent="0.3">
@@ -12677,10 +12719,10 @@
         <v>1025</v>
       </c>
       <c r="D490" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="E490" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.3">
@@ -12691,13 +12733,13 @@
         <v>6</v>
       </c>
       <c r="C491" t="s">
-        <v>1038</v>
+        <v>1025</v>
       </c>
       <c r="D491" t="s">
-        <v>1039</v>
+        <v>1032</v>
       </c>
       <c r="E491" t="s">
-        <v>1044</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.3">
@@ -12708,13 +12750,13 @@
         <v>6</v>
       </c>
       <c r="C492" t="s">
-        <v>1038</v>
+        <v>1025</v>
       </c>
       <c r="D492" t="s">
-        <v>1040</v>
+        <v>1158</v>
       </c>
       <c r="E492" t="s">
-        <v>1045</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.3">
@@ -12725,13 +12767,13 @@
         <v>6</v>
       </c>
       <c r="C493" t="s">
-        <v>1038</v>
+        <v>1025</v>
       </c>
       <c r="D493" t="s">
-        <v>1047</v>
+        <v>1157</v>
       </c>
       <c r="E493" t="s">
-        <v>1046</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.3">
@@ -12742,13 +12784,13 @@
         <v>6</v>
       </c>
       <c r="C494" t="s">
-        <v>1038</v>
+        <v>1025</v>
       </c>
       <c r="D494" t="s">
-        <v>1041</v>
+        <v>1033</v>
       </c>
       <c r="E494" t="s">
-        <v>1048</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.3">
@@ -12762,10 +12804,10 @@
         <v>1038</v>
       </c>
       <c r="D495" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="E495" t="s">
-        <v>1049</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.3">
@@ -12779,10 +12821,10 @@
         <v>1038</v>
       </c>
       <c r="D496" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="E496" t="s">
-        <v>1050</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.3">
@@ -12793,13 +12835,13 @@
         <v>6</v>
       </c>
       <c r="C497" t="s">
-        <v>1051</v>
+        <v>1038</v>
       </c>
       <c r="D497" t="s">
-        <v>1052</v>
+        <v>1047</v>
       </c>
       <c r="E497" t="s">
-        <v>1059</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="498" spans="1:5" x14ac:dyDescent="0.3">
@@ -12810,13 +12852,13 @@
         <v>6</v>
       </c>
       <c r="C498" t="s">
-        <v>1051</v>
+        <v>1038</v>
       </c>
       <c r="D498" t="s">
-        <v>1053</v>
+        <v>1041</v>
       </c>
       <c r="E498" t="s">
-        <v>1060</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="499" spans="1:5" x14ac:dyDescent="0.3">
@@ -12827,13 +12869,13 @@
         <v>6</v>
       </c>
       <c r="C499" t="s">
-        <v>1051</v>
+        <v>1038</v>
       </c>
       <c r="D499" t="s">
-        <v>1054</v>
+        <v>1042</v>
       </c>
       <c r="E499" t="s">
-        <v>1061</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.3">
@@ -12844,13 +12886,13 @@
         <v>6</v>
       </c>
       <c r="C500" t="s">
-        <v>1051</v>
+        <v>1038</v>
       </c>
       <c r="D500" t="s">
-        <v>1055</v>
+        <v>1043</v>
       </c>
       <c r="E500" t="s">
-        <v>1062</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="501" spans="1:5" x14ac:dyDescent="0.3">
@@ -12864,10 +12906,10 @@
         <v>1051</v>
       </c>
       <c r="D501" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="E501" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="502" spans="1:5" x14ac:dyDescent="0.3">
@@ -12881,10 +12923,10 @@
         <v>1051</v>
       </c>
       <c r="D502" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="E502" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.3">
@@ -12898,10 +12940,10 @@
         <v>1051</v>
       </c>
       <c r="D503" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="E503" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.3">
@@ -12912,13 +12954,13 @@
         <v>6</v>
       </c>
       <c r="C504" t="s">
-        <v>1066</v>
+        <v>1051</v>
       </c>
       <c r="D504" t="s">
-        <v>1067</v>
+        <v>1055</v>
       </c>
       <c r="E504" t="s">
-        <v>1073</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.3">
@@ -12929,13 +12971,13 @@
         <v>6</v>
       </c>
       <c r="C505" t="s">
-        <v>1066</v>
+        <v>1051</v>
       </c>
       <c r="D505" t="s">
-        <v>1068</v>
+        <v>1056</v>
       </c>
       <c r="E505" t="s">
-        <v>1074</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.3">
@@ -12946,13 +12988,13 @@
         <v>6</v>
       </c>
       <c r="C506" t="s">
-        <v>1066</v>
+        <v>1051</v>
       </c>
       <c r="D506" t="s">
-        <v>1069</v>
+        <v>1057</v>
       </c>
       <c r="E506" t="s">
-        <v>1075</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.3">
@@ -12963,13 +13005,13 @@
         <v>6</v>
       </c>
       <c r="C507" t="s">
-        <v>1066</v>
+        <v>1051</v>
       </c>
       <c r="D507" t="s">
-        <v>1070</v>
+        <v>1058</v>
       </c>
       <c r="E507" t="s">
-        <v>1076</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.3">
@@ -12983,10 +13025,10 @@
         <v>1066</v>
       </c>
       <c r="D508" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="E508" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.3">
@@ -13000,10 +13042,10 @@
         <v>1066</v>
       </c>
       <c r="D509" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="E509" t="s">
-        <v>1065</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.3">
@@ -13014,13 +13056,13 @@
         <v>6</v>
       </c>
       <c r="C510" t="s">
-        <v>1078</v>
+        <v>1066</v>
       </c>
       <c r="D510" t="s">
-        <v>1079</v>
+        <v>1069</v>
       </c>
       <c r="E510" t="s">
-        <v>1090</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.3">
@@ -13031,13 +13073,13 @@
         <v>6</v>
       </c>
       <c r="C511" t="s">
-        <v>1078</v>
+        <v>1066</v>
       </c>
       <c r="D511" t="s">
-        <v>1080</v>
+        <v>1070</v>
       </c>
       <c r="E511" t="s">
-        <v>1089</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.3">
@@ -13048,13 +13090,13 @@
         <v>6</v>
       </c>
       <c r="C512" t="s">
-        <v>1078</v>
+        <v>1066</v>
       </c>
       <c r="D512" t="s">
-        <v>1081</v>
+        <v>1071</v>
       </c>
       <c r="E512" t="s">
-        <v>1088</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.3">
@@ -13065,13 +13107,13 @@
         <v>6</v>
       </c>
       <c r="C513" t="s">
-        <v>1078</v>
+        <v>1066</v>
       </c>
       <c r="D513" t="s">
-        <v>1082</v>
+        <v>1153</v>
       </c>
       <c r="E513" t="s">
-        <v>1087</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.3">
@@ -13082,13 +13124,13 @@
         <v>6</v>
       </c>
       <c r="C514" t="s">
-        <v>1078</v>
+        <v>1066</v>
       </c>
       <c r="D514" t="s">
-        <v>1083</v>
+        <v>1154</v>
       </c>
       <c r="E514" t="s">
-        <v>1086</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.3">
@@ -13099,13 +13141,13 @@
         <v>6</v>
       </c>
       <c r="C515" t="s">
-        <v>1078</v>
+        <v>1066</v>
       </c>
       <c r="D515" t="s">
-        <v>1084</v>
+        <v>1072</v>
       </c>
       <c r="E515" t="s">
-        <v>1085</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.3">
@@ -13116,13 +13158,13 @@
         <v>6</v>
       </c>
       <c r="C516" t="s">
-        <v>1091</v>
+        <v>1078</v>
       </c>
       <c r="D516" t="s">
-        <v>1092</v>
+        <v>1079</v>
       </c>
       <c r="E516" t="s">
-        <v>1098</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="517" spans="1:5" x14ac:dyDescent="0.3">
@@ -13133,13 +13175,13 @@
         <v>6</v>
       </c>
       <c r="C517" t="s">
-        <v>1091</v>
+        <v>1078</v>
       </c>
       <c r="D517" t="s">
-        <v>1093</v>
+        <v>1080</v>
       </c>
       <c r="E517" t="s">
-        <v>1099</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.3">
@@ -13150,13 +13192,13 @@
         <v>6</v>
       </c>
       <c r="C518" t="s">
-        <v>1091</v>
+        <v>1078</v>
       </c>
       <c r="D518" t="s">
-        <v>1094</v>
+        <v>1081</v>
       </c>
       <c r="E518" t="s">
-        <v>1100</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.3">
@@ -13167,13 +13209,13 @@
         <v>6</v>
       </c>
       <c r="C519" t="s">
-        <v>1091</v>
+        <v>1078</v>
       </c>
       <c r="D519" t="s">
-        <v>1095</v>
+        <v>1082</v>
       </c>
       <c r="E519" t="s">
-        <v>1101</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="520" spans="1:5" x14ac:dyDescent="0.3">
@@ -13184,13 +13226,13 @@
         <v>6</v>
       </c>
       <c r="C520" t="s">
-        <v>1091</v>
+        <v>1078</v>
       </c>
       <c r="D520" t="s">
-        <v>1096</v>
+        <v>1083</v>
       </c>
       <c r="E520" t="s">
-        <v>1103</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="521" spans="1:5" x14ac:dyDescent="0.3">
@@ -13201,13 +13243,13 @@
         <v>6</v>
       </c>
       <c r="C521" t="s">
-        <v>1091</v>
+        <v>1078</v>
       </c>
       <c r="D521" t="s">
-        <v>1102</v>
+        <v>1152</v>
       </c>
       <c r="E521" t="s">
-        <v>1104</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.3">
@@ -13218,13 +13260,13 @@
         <v>6</v>
       </c>
       <c r="C522" t="s">
-        <v>1091</v>
+        <v>1078</v>
       </c>
       <c r="D522" t="s">
-        <v>1097</v>
+        <v>1084</v>
       </c>
       <c r="E522" t="s">
-        <v>1105</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.3">
@@ -13235,13 +13277,13 @@
         <v>6</v>
       </c>
       <c r="C523" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="D523" t="s">
-        <v>1107</v>
+        <v>1092</v>
       </c>
       <c r="E523" t="s">
-        <v>1114</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.3">
@@ -13252,13 +13294,13 @@
         <v>6</v>
       </c>
       <c r="C524" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="D524" t="s">
-        <v>1108</v>
+        <v>1093</v>
       </c>
       <c r="E524" t="s">
-        <v>1120</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.3">
@@ -13269,13 +13311,13 @@
         <v>6</v>
       </c>
       <c r="C525" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="D525" t="s">
-        <v>1109</v>
+        <v>1094</v>
       </c>
       <c r="E525" t="s">
-        <v>1115</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.3">
@@ -13286,13 +13328,13 @@
         <v>6</v>
       </c>
       <c r="C526" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="D526" t="s">
-        <v>1110</v>
+        <v>1095</v>
       </c>
       <c r="E526" t="s">
-        <v>1116</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.3">
@@ -13303,13 +13345,13 @@
         <v>6</v>
       </c>
       <c r="C527" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="D527" t="s">
-        <v>1111</v>
+        <v>1096</v>
       </c>
       <c r="E527" t="s">
-        <v>1117</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.3">
@@ -13320,13 +13362,13 @@
         <v>6</v>
       </c>
       <c r="C528" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="D528" t="s">
-        <v>1112</v>
+        <v>1102</v>
       </c>
       <c r="E528" t="s">
-        <v>1118</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.3">
@@ -13337,13 +13379,13 @@
         <v>6</v>
       </c>
       <c r="C529" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="D529" t="s">
-        <v>1113</v>
+        <v>1097</v>
       </c>
       <c r="E529" t="s">
-        <v>1119</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.3">
@@ -13354,13 +13396,13 @@
         <v>6</v>
       </c>
       <c r="C530" t="s">
-        <v>1121</v>
+        <v>1106</v>
       </c>
       <c r="D530" t="s">
-        <v>1122</v>
+        <v>1107</v>
       </c>
       <c r="E530" t="s">
-        <v>1129</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.3">
@@ -13371,13 +13413,13 @@
         <v>6</v>
       </c>
       <c r="C531" t="s">
-        <v>1121</v>
+        <v>1106</v>
       </c>
       <c r="D531" t="s">
-        <v>1123</v>
+        <v>1108</v>
       </c>
       <c r="E531" t="s">
-        <v>1130</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="532" spans="1:5" x14ac:dyDescent="0.3">
@@ -13388,13 +13430,13 @@
         <v>6</v>
       </c>
       <c r="C532" t="s">
-        <v>1121</v>
+        <v>1106</v>
       </c>
       <c r="D532" t="s">
-        <v>1124</v>
+        <v>1109</v>
       </c>
       <c r="E532" t="s">
-        <v>1131</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.3">
@@ -13405,13 +13447,13 @@
         <v>6</v>
       </c>
       <c r="C533" t="s">
-        <v>1121</v>
+        <v>1106</v>
       </c>
       <c r="D533" t="s">
-        <v>1125</v>
+        <v>1110</v>
       </c>
       <c r="E533" t="s">
-        <v>1132</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.3">
@@ -13422,13 +13464,13 @@
         <v>6</v>
       </c>
       <c r="C534" t="s">
-        <v>1121</v>
+        <v>1106</v>
       </c>
       <c r="D534" t="s">
-        <v>1126</v>
+        <v>1111</v>
       </c>
       <c r="E534" t="s">
-        <v>1133</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.3">
@@ -13439,13 +13481,13 @@
         <v>6</v>
       </c>
       <c r="C535" t="s">
-        <v>1121</v>
+        <v>1106</v>
       </c>
       <c r="D535" t="s">
-        <v>1127</v>
+        <v>1112</v>
       </c>
       <c r="E535" t="s">
-        <v>1134</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="536" spans="1:5" x14ac:dyDescent="0.3">
@@ -13456,13 +13498,13 @@
         <v>6</v>
       </c>
       <c r="C536" t="s">
-        <v>1121</v>
+        <v>1106</v>
       </c>
       <c r="D536" t="s">
-        <v>1128</v>
+        <v>1113</v>
       </c>
       <c r="E536" t="s">
-        <v>1135</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="537" spans="1:5" x14ac:dyDescent="0.3">
@@ -13473,13 +13515,13 @@
         <v>6</v>
       </c>
       <c r="C537" t="s">
-        <v>1136</v>
+        <v>1121</v>
       </c>
       <c r="D537" t="s">
-        <v>1137</v>
+        <v>1122</v>
       </c>
       <c r="E537" t="s">
-        <v>1143</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.3">
@@ -13490,13 +13532,13 @@
         <v>6</v>
       </c>
       <c r="C538" t="s">
-        <v>1136</v>
+        <v>1121</v>
       </c>
       <c r="D538" t="s">
-        <v>1146</v>
+        <v>1123</v>
       </c>
       <c r="E538" t="s">
-        <v>1144</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="539" spans="1:5" x14ac:dyDescent="0.3">
@@ -13507,13 +13549,13 @@
         <v>6</v>
       </c>
       <c r="C539" t="s">
-        <v>1136</v>
+        <v>1121</v>
       </c>
       <c r="D539" t="s">
-        <v>1138</v>
+        <v>1124</v>
       </c>
       <c r="E539" t="s">
-        <v>1145</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="540" spans="1:5" x14ac:dyDescent="0.3">
@@ -13524,13 +13566,13 @@
         <v>6</v>
       </c>
       <c r="C540" t="s">
-        <v>1136</v>
+        <v>1121</v>
       </c>
       <c r="D540" t="s">
-        <v>1139</v>
+        <v>1125</v>
       </c>
       <c r="E540" t="s">
-        <v>1147</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.3">
@@ -13541,13 +13583,13 @@
         <v>6</v>
       </c>
       <c r="C541" t="s">
-        <v>1136</v>
+        <v>1121</v>
       </c>
       <c r="D541" t="s">
-        <v>1140</v>
+        <v>1126</v>
       </c>
       <c r="E541" t="s">
-        <v>1148</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.3">
@@ -13558,13 +13600,13 @@
         <v>6</v>
       </c>
       <c r="C542" t="s">
-        <v>1136</v>
+        <v>1121</v>
       </c>
       <c r="D542" t="s">
-        <v>1141</v>
+        <v>1127</v>
       </c>
       <c r="E542" t="s">
-        <v>1149</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.3">
@@ -13575,13 +13617,13 @@
         <v>6</v>
       </c>
       <c r="C543" t="s">
-        <v>1136</v>
+        <v>1121</v>
       </c>
       <c r="D543" t="s">
-        <v>1142</v>
+        <v>1128</v>
       </c>
       <c r="E543" t="s">
-        <v>1150</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.3">
@@ -13591,69 +13633,116 @@
       <c r="B544" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="545" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C544" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D544" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E544" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="545" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A545" t="s">
         <v>5</v>
       </c>
       <c r="B545" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="546" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C545" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D545" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E545" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="546" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A546" t="s">
         <v>5</v>
       </c>
       <c r="B546" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="547" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C546" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D546" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E546" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="547" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
         <v>5</v>
       </c>
       <c r="B547" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="548" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C547" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D547" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E547" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="548" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A548" t="s">
         <v>5</v>
       </c>
       <c r="B548" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="549" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C548" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D548" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E548" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="549" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A549" t="s">
         <v>5</v>
       </c>
       <c r="B549" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="550" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C549" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D549" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E549" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="550" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A550" t="s">
         <v>5</v>
       </c>
       <c r="B550" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="551" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A551" t="s">
-        <v>5</v>
-      </c>
-      <c r="B551" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="552" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A552" t="s">
-        <v>5</v>
-      </c>
-      <c r="B552" t="s">
-        <v>6</v>
+      <c r="C550" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D550" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E550" t="s">
+        <v>1150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodato jos 13 u prvu i sve u drugu fazu: Dusan
</commit_message>
<xml_diff>
--- a/faza1_tabela.xlsx
+++ b/faza1_tabela.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duja0807\Desktop\master\natural_project\natural-language-processing-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE910CFD-98CC-4BF3-BAC6-C8164933F9FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04296586-7748-44D7-B2B1-96D882DBFF7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14310" yWindow="-105" windowWidth="28995" windowHeight="15795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3524" uniqueCount="1539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="1565">
   <si>
     <t>ProgrammingLanguageName</t>
   </si>
@@ -4637,6 +4637,84 @@
   </si>
   <si>
     <t xml:space="preserve">  Brise sve SEO linkove za neki indexirani objekat  </t>
+  </si>
+  <si>
+    <t>40_addCollector</t>
+  </si>
+  <si>
+    <t>40_addPath</t>
+  </si>
+  <si>
+    <t>40_attachCallback</t>
+  </si>
+  <si>
+    <t>40_check_credentials</t>
+  </si>
+  <si>
+    <t>40_entityToString</t>
+  </si>
+  <si>
+    <t>40_extractEnumFromArray</t>
+  </si>
+  <si>
+    <t>40_findInternal</t>
+  </si>
+  <si>
+    <t>40_findValueTypeName</t>
+  </si>
+  <si>
+    <t>40_getAllEnumTags</t>
+  </si>
+  <si>
+    <t>40_getDynamicFunc</t>
+  </si>
+  <si>
+    <t>40_getEnumByID</t>
+  </si>
+  <si>
+    <t>40_getEnumName</t>
+  </si>
+  <si>
+    <t>40_getThemeConfig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Dodaje zadati sakupljac u prioritetni red uz  dodatne provere i bacanje izuzetaka  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Dodaje putanju u predefinisani niz koja ce  moci da se koristi nakon upisa u fajl  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Postavlja callback funkciju u prioritetni red  u zavisnosti od zadatog prioriteta ako nije podrazumevani  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Proverava kredencijale korisnickog imena i lozinke  i inicijalizuje i postavlja sesiju za dalje koriscenje  u kukije  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Pretvara dati objekat u niz stringova razdvojenih  postavljenim separatorom  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Pronalazi ime za enum u nizu vrednosti  za zadati parametar u zavisnosti od korisnika   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Pronalazi listu unutrasnjih klasa definisanih unutar  prosledjene okruzujuce klase  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ova funkcija dohvata tip po zadataoj  vrednosti enum ako je ona validno definisana  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Pronalazi sve tagove za odredjeni enum po njegovom id  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Pronalazi dinamicki definisane funkcije i smesta  ih u listu za dalju obradu u klasama  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Dohvata ime enum za zadati ID polja koje mu  pripada ukoliko je definisano  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Vraca ime enum tipa za zadatu vrednost proizvoda  kao jedinog parametra funkcije   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Uzima podesavanja za odredjenu temu i uz odredjene provere  pronalazi putanju do trazenog fajla  </t>
   </si>
 </sst>
 </file>
@@ -5504,8 +5582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E750"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A331" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D351" sqref="D351"/>
+    <sheetView tabSelected="1" topLeftCell="C541" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E359" sqref="E359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11474,6 +11552,12 @@
       <c r="B351" t="s">
         <v>6</v>
       </c>
+      <c r="D351" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E351" t="s">
+        <v>1552</v>
+      </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
@@ -11482,6 +11566,12 @@
       <c r="B352" t="s">
         <v>6</v>
       </c>
+      <c r="D352" t="s">
+        <v>1540</v>
+      </c>
+      <c r="E352" t="s">
+        <v>1553</v>
+      </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
@@ -11490,6 +11580,12 @@
       <c r="B353" t="s">
         <v>6</v>
       </c>
+      <c r="D353" t="s">
+        <v>1541</v>
+      </c>
+      <c r="E353" t="s">
+        <v>1554</v>
+      </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
@@ -11498,6 +11594,12 @@
       <c r="B354" t="s">
         <v>6</v>
       </c>
+      <c r="D354" t="s">
+        <v>1542</v>
+      </c>
+      <c r="E354" t="s">
+        <v>1555</v>
+      </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
@@ -11506,6 +11608,12 @@
       <c r="B355" t="s">
         <v>6</v>
       </c>
+      <c r="D355" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E355" t="s">
+        <v>1556</v>
+      </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
@@ -11514,6 +11622,12 @@
       <c r="B356" t="s">
         <v>6</v>
       </c>
+      <c r="D356" t="s">
+        <v>1544</v>
+      </c>
+      <c r="E356" t="s">
+        <v>1557</v>
+      </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
@@ -11522,6 +11636,12 @@
       <c r="B357" t="s">
         <v>6</v>
       </c>
+      <c r="D357" t="s">
+        <v>1545</v>
+      </c>
+      <c r="E357" t="s">
+        <v>1558</v>
+      </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
@@ -11530,6 +11650,12 @@
       <c r="B358" t="s">
         <v>6</v>
       </c>
+      <c r="D358" t="s">
+        <v>1546</v>
+      </c>
+      <c r="E358" t="s">
+        <v>1559</v>
+      </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
@@ -11538,6 +11664,12 @@
       <c r="B359" t="s">
         <v>6</v>
       </c>
+      <c r="D359" t="s">
+        <v>1547</v>
+      </c>
+      <c r="E359" t="s">
+        <v>1560</v>
+      </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
@@ -11546,6 +11678,12 @@
       <c r="B360" t="s">
         <v>6</v>
       </c>
+      <c r="D360" t="s">
+        <v>1548</v>
+      </c>
+      <c r="E360" t="s">
+        <v>1561</v>
+      </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
@@ -11554,6 +11692,12 @@
       <c r="B361" t="s">
         <v>6</v>
       </c>
+      <c r="D361" t="s">
+        <v>1549</v>
+      </c>
+      <c r="E361" t="s">
+        <v>1562</v>
+      </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
@@ -11562,6 +11706,12 @@
       <c r="B362" t="s">
         <v>6</v>
       </c>
+      <c r="D362" t="s">
+        <v>1550</v>
+      </c>
+      <c r="E362" t="s">
+        <v>1563</v>
+      </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
@@ -11569,6 +11719,12 @@
       </c>
       <c r="B363" t="s">
         <v>6</v>
+      </c>
+      <c r="D363" t="s">
+        <v>1551</v>
+      </c>
+      <c r="E363" t="s">
+        <v>1564</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Eksel faza_1: dodati opisi u koloni Source desc od 40-70
Eksel faza_2: samo izmena nekih slova C kao Cirilo i Metodije u tekstu upita
</commit_message>
<xml_diff>
--- a/faza1_tabela.xlsx
+++ b/faza1_tabela.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duja0807\Desktop\master\natural_project\natural-language-processing-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F348D24-FFCD-4823-8A47-DE946A681913}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994148C6-5E3B-4345-B525-172412985CD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="1566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3750" uniqueCount="1597">
   <si>
     <t>ProgrammingLanguageName</t>
   </si>
@@ -4718,6 +4718,99 @@
   </si>
   <si>
     <t>Proverava da je sortString dobro formatiran i dodaje uslov   za sortiranje definisano u query   Vraca i poruku http strani o nekorektnom formatu za sortiranje stringova</t>
+  </si>
+  <si>
+    <t>Fajlovi sa pomocnim klasama i enumeracijama.</t>
+  </si>
+  <si>
+    <t>Pomocne klase za obradu parametara i kordiranje urla.</t>
+  </si>
+  <si>
+    <t>Funkcije za slanje i obradu api poziva uz koriscenje kolacica</t>
+  </si>
+  <si>
+    <t>Util klase za obradu nizova.</t>
+  </si>
+  <si>
+    <t>Razne funkcije za obradu datuma.</t>
+  </si>
+  <si>
+    <t>Funkcije za dodatnu obradu html elemenata.</t>
+  </si>
+  <si>
+    <t>Metode za obradu nizova razlicitih objekata.</t>
+  </si>
+  <si>
+    <t>Util funkcije za obradu stringova.</t>
+  </si>
+  <si>
+    <t>Klase za rad sa fajlovima.</t>
+  </si>
+  <si>
+    <t>Operacije nad clipboardom.</t>
+  </si>
+  <si>
+    <t>Funkcije za konverziju tipova fajlova.</t>
+  </si>
+  <si>
+    <t>Metode za konvertovanje json fajlova.</t>
+  </si>
+  <si>
+    <t>Funkcije za generisanje nasumicnih vrednosti.</t>
+  </si>
+  <si>
+    <t>Klase za obradu grafova.</t>
+  </si>
+  <si>
+    <t>Optimizacija nelder mead algoritmom.</t>
+  </si>
+  <si>
+    <t>Funkcije za brojanje jedinstvenih elemenata koriscenjem skupa.</t>
+  </si>
+  <si>
+    <t>Obrada podataka i tabela u bazi podataka.</t>
+  </si>
+  <si>
+    <t>Metode za deserijalizaciju jsona.</t>
+  </si>
+  <si>
+    <t>Funkcije za obradu i parsiranje stringa.</t>
+  </si>
+  <si>
+    <t>Klase za obradjivanje niti i procesa.</t>
+  </si>
+  <si>
+    <t>Pomocne funkcije za obradu stringova regularnim izrazima.</t>
+  </si>
+  <si>
+    <t>Funkcije za pravljenje http odgovora.</t>
+  </si>
+  <si>
+    <t>Pomocne metode za validaciju stringa.</t>
+  </si>
+  <si>
+    <t>Metode za preslikavanje entiteta u html.</t>
+  </si>
+  <si>
+    <t>Funkcije za operacije nad fajlovima.</t>
+  </si>
+  <si>
+    <t>Pomocne funkcije za obradu i sortiranje nizova.</t>
+  </si>
+  <si>
+    <t>Fajlovi za obradu stringova naprednijim metodama.</t>
+  </si>
+  <si>
+    <t>Funkcije za obradu htmla.</t>
+  </si>
+  <si>
+    <t>Pomocne klase za obradu tekstova iz fajlova.</t>
+  </si>
+  <si>
+    <t>Klase za eknkriptovanje raznim algoritmima.</t>
+  </si>
+  <si>
+    <t>Pomocne metode za matematicke obrade nizova i matrica.</t>
   </si>
 </sst>
 </file>
@@ -5585,8 +5678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E750"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C327" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D351" sqref="D351:D550"/>
+    <sheetView tabSelected="1" topLeftCell="B524" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C542" sqref="C542"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11555,6 +11648,9 @@
       <c r="B351" t="s">
         <v>6</v>
       </c>
+      <c r="C351" t="s">
+        <v>1566</v>
+      </c>
       <c r="D351" t="s">
         <v>1329</v>
       </c>
@@ -11569,6 +11665,9 @@
       <c r="B352" t="s">
         <v>6</v>
       </c>
+      <c r="C352" t="s">
+        <v>1566</v>
+      </c>
       <c r="D352" t="s">
         <v>1330</v>
       </c>
@@ -11583,6 +11682,9 @@
       <c r="B353" t="s">
         <v>6</v>
       </c>
+      <c r="C353" t="s">
+        <v>1566</v>
+      </c>
       <c r="D353" t="s">
         <v>1331</v>
       </c>
@@ -11597,6 +11699,9 @@
       <c r="B354" t="s">
         <v>6</v>
       </c>
+      <c r="C354" t="s">
+        <v>1566</v>
+      </c>
       <c r="D354" t="s">
         <v>1332</v>
       </c>
@@ -11611,6 +11716,9 @@
       <c r="B355" t="s">
         <v>6</v>
       </c>
+      <c r="C355" t="s">
+        <v>1566</v>
+      </c>
       <c r="D355" t="s">
         <v>1333</v>
       </c>
@@ -11625,6 +11733,9 @@
       <c r="B356" t="s">
         <v>6</v>
       </c>
+      <c r="C356" t="s">
+        <v>1566</v>
+      </c>
       <c r="D356" t="s">
         <v>1334</v>
       </c>
@@ -11639,6 +11750,9 @@
       <c r="B357" t="s">
         <v>6</v>
       </c>
+      <c r="C357" t="s">
+        <v>1566</v>
+      </c>
       <c r="D357" t="s">
         <v>1335</v>
       </c>
@@ -11653,6 +11767,9 @@
       <c r="B358" t="s">
         <v>6</v>
       </c>
+      <c r="C358" t="s">
+        <v>1566</v>
+      </c>
       <c r="D358" t="s">
         <v>1336</v>
       </c>
@@ -11667,6 +11784,9 @@
       <c r="B359" t="s">
         <v>6</v>
       </c>
+      <c r="C359" t="s">
+        <v>1566</v>
+      </c>
       <c r="D359" t="s">
         <v>1337</v>
       </c>
@@ -11681,6 +11801,9 @@
       <c r="B360" t="s">
         <v>6</v>
       </c>
+      <c r="C360" t="s">
+        <v>1566</v>
+      </c>
       <c r="D360" t="s">
         <v>1338</v>
       </c>
@@ -11695,6 +11818,9 @@
       <c r="B361" t="s">
         <v>6</v>
       </c>
+      <c r="C361" t="s">
+        <v>1566</v>
+      </c>
       <c r="D361" t="s">
         <v>1339</v>
       </c>
@@ -11709,6 +11835,9 @@
       <c r="B362" t="s">
         <v>6</v>
       </c>
+      <c r="C362" t="s">
+        <v>1566</v>
+      </c>
       <c r="D362" t="s">
         <v>1340</v>
       </c>
@@ -11723,6 +11852,9 @@
       <c r="B363" t="s">
         <v>6</v>
       </c>
+      <c r="C363" t="s">
+        <v>1566</v>
+      </c>
       <c r="D363" t="s">
         <v>1341</v>
       </c>
@@ -11737,6 +11869,9 @@
       <c r="B364" t="s">
         <v>6</v>
       </c>
+      <c r="C364" t="s">
+        <v>1567</v>
+      </c>
       <c r="D364" t="s">
         <v>1142</v>
       </c>
@@ -11751,6 +11886,9 @@
       <c r="B365" t="s">
         <v>6</v>
       </c>
+      <c r="C365" t="s">
+        <v>1567</v>
+      </c>
       <c r="D365" t="s">
         <v>1143</v>
       </c>
@@ -11765,6 +11903,9 @@
       <c r="B366" t="s">
         <v>6</v>
       </c>
+      <c r="C366" t="s">
+        <v>1567</v>
+      </c>
       <c r="D366" t="s">
         <v>1144</v>
       </c>
@@ -11779,6 +11920,9 @@
       <c r="B367" t="s">
         <v>6</v>
       </c>
+      <c r="C367" t="s">
+        <v>1567</v>
+      </c>
       <c r="D367" t="s">
         <v>1145</v>
       </c>
@@ -11793,6 +11937,9 @@
       <c r="B368" t="s">
         <v>6</v>
       </c>
+      <c r="C368" t="s">
+        <v>1567</v>
+      </c>
       <c r="D368" t="s">
         <v>1146</v>
       </c>
@@ -11807,6 +11954,9 @@
       <c r="B369" t="s">
         <v>6</v>
       </c>
+      <c r="C369" t="s">
+        <v>1567</v>
+      </c>
       <c r="D369" t="s">
         <v>1147</v>
       </c>
@@ -11821,6 +11971,9 @@
       <c r="B370" t="s">
         <v>6</v>
       </c>
+      <c r="C370" t="s">
+        <v>1567</v>
+      </c>
       <c r="D370" t="s">
         <v>1148</v>
       </c>
@@ -11835,6 +11988,9 @@
       <c r="B371" t="s">
         <v>6</v>
       </c>
+      <c r="C371" t="s">
+        <v>1568</v>
+      </c>
       <c r="D371" t="s">
         <v>1149</v>
       </c>
@@ -11849,6 +12005,9 @@
       <c r="B372" t="s">
         <v>6</v>
       </c>
+      <c r="C372" t="s">
+        <v>1568</v>
+      </c>
       <c r="D372" t="s">
         <v>1150</v>
       </c>
@@ -11863,6 +12022,9 @@
       <c r="B373" t="s">
         <v>6</v>
       </c>
+      <c r="C373" t="s">
+        <v>1568</v>
+      </c>
       <c r="D373" t="s">
         <v>1151</v>
       </c>
@@ -11877,6 +12039,9 @@
       <c r="B374" t="s">
         <v>6</v>
       </c>
+      <c r="C374" t="s">
+        <v>1568</v>
+      </c>
       <c r="D374" t="s">
         <v>1152</v>
       </c>
@@ -11891,6 +12056,9 @@
       <c r="B375" t="s">
         <v>6</v>
       </c>
+      <c r="C375" t="s">
+        <v>1568</v>
+      </c>
       <c r="D375" t="s">
         <v>1153</v>
       </c>
@@ -11905,6 +12073,9 @@
       <c r="B376" t="s">
         <v>6</v>
       </c>
+      <c r="C376" t="s">
+        <v>1568</v>
+      </c>
       <c r="D376" t="s">
         <v>1154</v>
       </c>
@@ -11919,6 +12090,9 @@
       <c r="B377" t="s">
         <v>6</v>
       </c>
+      <c r="C377" t="s">
+        <v>1568</v>
+      </c>
       <c r="D377" t="s">
         <v>1155</v>
       </c>
@@ -11933,6 +12107,9 @@
       <c r="B378" t="s">
         <v>6</v>
       </c>
+      <c r="C378" t="s">
+        <v>1569</v>
+      </c>
       <c r="D378" t="s">
         <v>1156</v>
       </c>
@@ -11947,6 +12124,9 @@
       <c r="B379" t="s">
         <v>6</v>
       </c>
+      <c r="C379" t="s">
+        <v>1569</v>
+      </c>
       <c r="D379" t="s">
         <v>1157</v>
       </c>
@@ -11961,6 +12141,9 @@
       <c r="B380" t="s">
         <v>6</v>
       </c>
+      <c r="C380" t="s">
+        <v>1569</v>
+      </c>
       <c r="D380" t="s">
         <v>1158</v>
       </c>
@@ -11975,6 +12158,9 @@
       <c r="B381" t="s">
         <v>6</v>
       </c>
+      <c r="C381" t="s">
+        <v>1569</v>
+      </c>
       <c r="D381" t="s">
         <v>1159</v>
       </c>
@@ -11989,6 +12175,9 @@
       <c r="B382" t="s">
         <v>6</v>
       </c>
+      <c r="C382" t="s">
+        <v>1569</v>
+      </c>
       <c r="D382" t="s">
         <v>1160</v>
       </c>
@@ -12003,6 +12192,9 @@
       <c r="B383" t="s">
         <v>6</v>
       </c>
+      <c r="C383" t="s">
+        <v>1569</v>
+      </c>
       <c r="D383" t="s">
         <v>1161</v>
       </c>
@@ -12017,6 +12209,9 @@
       <c r="B384" t="s">
         <v>6</v>
       </c>
+      <c r="C384" t="s">
+        <v>1570</v>
+      </c>
       <c r="D384" t="s">
         <v>1162</v>
       </c>
@@ -12031,6 +12226,9 @@
       <c r="B385" t="s">
         <v>6</v>
       </c>
+      <c r="C385" t="s">
+        <v>1570</v>
+      </c>
       <c r="D385" t="s">
         <v>1163</v>
       </c>
@@ -12045,6 +12243,9 @@
       <c r="B386" t="s">
         <v>6</v>
       </c>
+      <c r="C386" t="s">
+        <v>1570</v>
+      </c>
       <c r="D386" t="s">
         <v>1164</v>
       </c>
@@ -12059,6 +12260,9 @@
       <c r="B387" t="s">
         <v>6</v>
       </c>
+      <c r="C387" t="s">
+        <v>1570</v>
+      </c>
       <c r="D387" t="s">
         <v>1165</v>
       </c>
@@ -12073,6 +12277,9 @@
       <c r="B388" t="s">
         <v>6</v>
       </c>
+      <c r="C388" t="s">
+        <v>1570</v>
+      </c>
       <c r="D388" t="s">
         <v>1166</v>
       </c>
@@ -12087,6 +12294,9 @@
       <c r="B389" t="s">
         <v>6</v>
       </c>
+      <c r="C389" t="s">
+        <v>1570</v>
+      </c>
       <c r="D389" t="s">
         <v>1167</v>
       </c>
@@ -12101,6 +12311,9 @@
       <c r="B390" t="s">
         <v>6</v>
       </c>
+      <c r="C390" t="s">
+        <v>1571</v>
+      </c>
       <c r="D390" t="s">
         <v>1168</v>
       </c>
@@ -12115,6 +12328,9 @@
       <c r="B391" t="s">
         <v>6</v>
       </c>
+      <c r="C391" t="s">
+        <v>1571</v>
+      </c>
       <c r="D391" t="s">
         <v>1169</v>
       </c>
@@ -12129,6 +12345,9 @@
       <c r="B392" t="s">
         <v>6</v>
       </c>
+      <c r="C392" t="s">
+        <v>1571</v>
+      </c>
       <c r="D392" t="s">
         <v>1170</v>
       </c>
@@ -12143,6 +12362,9 @@
       <c r="B393" t="s">
         <v>6</v>
       </c>
+      <c r="C393" t="s">
+        <v>1571</v>
+      </c>
       <c r="D393" t="s">
         <v>1171</v>
       </c>
@@ -12157,6 +12379,9 @@
       <c r="B394" t="s">
         <v>6</v>
       </c>
+      <c r="C394" t="s">
+        <v>1571</v>
+      </c>
       <c r="D394" t="s">
         <v>1172</v>
       </c>
@@ -12171,6 +12396,9 @@
       <c r="B395" t="s">
         <v>6</v>
       </c>
+      <c r="C395" t="s">
+        <v>1571</v>
+      </c>
       <c r="D395" t="s">
         <v>1173</v>
       </c>
@@ -12185,6 +12413,9 @@
       <c r="B396" t="s">
         <v>6</v>
       </c>
+      <c r="C396" t="s">
+        <v>1572</v>
+      </c>
       <c r="D396" t="s">
         <v>1174</v>
       </c>
@@ -12199,6 +12430,9 @@
       <c r="B397" t="s">
         <v>6</v>
       </c>
+      <c r="C397" t="s">
+        <v>1572</v>
+      </c>
       <c r="D397" t="s">
         <v>1175</v>
       </c>
@@ -12213,6 +12447,9 @@
       <c r="B398" t="s">
         <v>6</v>
       </c>
+      <c r="C398" t="s">
+        <v>1572</v>
+      </c>
       <c r="D398" t="s">
         <v>1176</v>
       </c>
@@ -12227,6 +12464,9 @@
       <c r="B399" t="s">
         <v>6</v>
       </c>
+      <c r="C399" t="s">
+        <v>1572</v>
+      </c>
       <c r="D399" t="s">
         <v>1177</v>
       </c>
@@ -12241,6 +12481,9 @@
       <c r="B400" t="s">
         <v>6</v>
       </c>
+      <c r="C400" t="s">
+        <v>1572</v>
+      </c>
       <c r="D400" t="s">
         <v>1178</v>
       </c>
@@ -12255,6 +12498,9 @@
       <c r="B401" t="s">
         <v>6</v>
       </c>
+      <c r="C401" t="s">
+        <v>1572</v>
+      </c>
       <c r="D401" t="s">
         <v>1179</v>
       </c>
@@ -12269,6 +12515,9 @@
       <c r="B402" t="s">
         <v>6</v>
       </c>
+      <c r="C402" t="s">
+        <v>1573</v>
+      </c>
       <c r="D402" t="s">
         <v>1180</v>
       </c>
@@ -12283,6 +12532,9 @@
       <c r="B403" t="s">
         <v>6</v>
       </c>
+      <c r="C403" t="s">
+        <v>1573</v>
+      </c>
       <c r="D403" t="s">
         <v>1181</v>
       </c>
@@ -12297,6 +12549,9 @@
       <c r="B404" t="s">
         <v>6</v>
       </c>
+      <c r="C404" t="s">
+        <v>1573</v>
+      </c>
       <c r="D404" t="s">
         <v>1182</v>
       </c>
@@ -12311,6 +12566,9 @@
       <c r="B405" t="s">
         <v>6</v>
       </c>
+      <c r="C405" t="s">
+        <v>1573</v>
+      </c>
       <c r="D405" t="s">
         <v>1183</v>
       </c>
@@ -12325,6 +12583,9 @@
       <c r="B406" t="s">
         <v>6</v>
       </c>
+      <c r="C406" t="s">
+        <v>1573</v>
+      </c>
       <c r="D406" t="s">
         <v>1184</v>
       </c>
@@ -12339,6 +12600,9 @@
       <c r="B407" t="s">
         <v>6</v>
       </c>
+      <c r="C407" t="s">
+        <v>1573</v>
+      </c>
       <c r="D407" t="s">
         <v>1185</v>
       </c>
@@ -12353,6 +12617,9 @@
       <c r="B408" t="s">
         <v>6</v>
       </c>
+      <c r="C408" t="s">
+        <v>1574</v>
+      </c>
       <c r="D408" t="s">
         <v>1186</v>
       </c>
@@ -12367,6 +12634,9 @@
       <c r="B409" t="s">
         <v>6</v>
       </c>
+      <c r="C409" t="s">
+        <v>1574</v>
+      </c>
       <c r="D409" t="s">
         <v>1187</v>
       </c>
@@ -12381,6 +12651,9 @@
       <c r="B410" t="s">
         <v>6</v>
       </c>
+      <c r="C410" t="s">
+        <v>1574</v>
+      </c>
       <c r="D410" t="s">
         <v>1188</v>
       </c>
@@ -12395,6 +12668,9 @@
       <c r="B411" t="s">
         <v>6</v>
       </c>
+      <c r="C411" t="s">
+        <v>1574</v>
+      </c>
       <c r="D411" t="s">
         <v>1189</v>
       </c>
@@ -12409,6 +12685,9 @@
       <c r="B412" t="s">
         <v>6</v>
       </c>
+      <c r="C412" t="s">
+        <v>1574</v>
+      </c>
       <c r="D412" t="s">
         <v>1190</v>
       </c>
@@ -12423,6 +12702,9 @@
       <c r="B413" t="s">
         <v>6</v>
       </c>
+      <c r="C413" t="s">
+        <v>1574</v>
+      </c>
       <c r="D413" t="s">
         <v>1191</v>
       </c>
@@ -12437,6 +12719,9 @@
       <c r="B414" t="s">
         <v>6</v>
       </c>
+      <c r="C414" t="s">
+        <v>1575</v>
+      </c>
       <c r="D414" t="s">
         <v>1192</v>
       </c>
@@ -12451,6 +12736,9 @@
       <c r="B415" t="s">
         <v>6</v>
       </c>
+      <c r="C415" t="s">
+        <v>1575</v>
+      </c>
       <c r="D415" t="s">
         <v>1193</v>
       </c>
@@ -12465,6 +12753,9 @@
       <c r="B416" t="s">
         <v>6</v>
       </c>
+      <c r="C416" t="s">
+        <v>1575</v>
+      </c>
       <c r="D416" t="s">
         <v>1194</v>
       </c>
@@ -12479,6 +12770,9 @@
       <c r="B417" t="s">
         <v>6</v>
       </c>
+      <c r="C417" t="s">
+        <v>1575</v>
+      </c>
       <c r="D417" t="s">
         <v>1195</v>
       </c>
@@ -12493,6 +12787,9 @@
       <c r="B418" t="s">
         <v>6</v>
       </c>
+      <c r="C418" t="s">
+        <v>1575</v>
+      </c>
       <c r="D418" t="s">
         <v>1196</v>
       </c>
@@ -12507,6 +12804,9 @@
       <c r="B419" t="s">
         <v>6</v>
       </c>
+      <c r="C419" t="s">
+        <v>1575</v>
+      </c>
       <c r="D419" t="s">
         <v>1197</v>
       </c>
@@ -12521,6 +12821,9 @@
       <c r="B420" t="s">
         <v>6</v>
       </c>
+      <c r="C420" t="s">
+        <v>1576</v>
+      </c>
       <c r="D420" t="s">
         <v>1198</v>
       </c>
@@ -12535,6 +12838,9 @@
       <c r="B421" t="s">
         <v>6</v>
       </c>
+      <c r="C421" t="s">
+        <v>1576</v>
+      </c>
       <c r="D421" t="s">
         <v>1199</v>
       </c>
@@ -12549,6 +12855,9 @@
       <c r="B422" t="s">
         <v>6</v>
       </c>
+      <c r="C422" t="s">
+        <v>1576</v>
+      </c>
       <c r="D422" t="s">
         <v>1200</v>
       </c>
@@ -12563,6 +12872,9 @@
       <c r="B423" t="s">
         <v>6</v>
       </c>
+      <c r="C423" t="s">
+        <v>1576</v>
+      </c>
       <c r="D423" t="s">
         <v>1201</v>
       </c>
@@ -12577,6 +12889,9 @@
       <c r="B424" t="s">
         <v>6</v>
       </c>
+      <c r="C424" t="s">
+        <v>1576</v>
+      </c>
       <c r="D424" t="s">
         <v>1202</v>
       </c>
@@ -12591,6 +12906,9 @@
       <c r="B425" t="s">
         <v>6</v>
       </c>
+      <c r="C425" t="s">
+        <v>1577</v>
+      </c>
       <c r="D425" t="s">
         <v>1203</v>
       </c>
@@ -12605,6 +12923,9 @@
       <c r="B426" t="s">
         <v>6</v>
       </c>
+      <c r="C426" t="s">
+        <v>1577</v>
+      </c>
       <c r="D426" t="s">
         <v>1204</v>
       </c>
@@ -12619,6 +12940,9 @@
       <c r="B427" t="s">
         <v>6</v>
       </c>
+      <c r="C427" t="s">
+        <v>1577</v>
+      </c>
       <c r="D427" t="s">
         <v>1205</v>
       </c>
@@ -12633,6 +12957,9 @@
       <c r="B428" t="s">
         <v>6</v>
       </c>
+      <c r="C428" t="s">
+        <v>1577</v>
+      </c>
       <c r="D428" t="s">
         <v>1206</v>
       </c>
@@ -12647,6 +12974,9 @@
       <c r="B429" t="s">
         <v>6</v>
       </c>
+      <c r="C429" t="s">
+        <v>1577</v>
+      </c>
       <c r="D429" t="s">
         <v>1207</v>
       </c>
@@ -12661,6 +12991,9 @@
       <c r="B430" t="s">
         <v>6</v>
       </c>
+      <c r="C430" t="s">
+        <v>1577</v>
+      </c>
       <c r="D430" t="s">
         <v>1208</v>
       </c>
@@ -12675,6 +13008,9 @@
       <c r="B431" t="s">
         <v>6</v>
       </c>
+      <c r="C431" t="s">
+        <v>1578</v>
+      </c>
       <c r="D431" t="s">
         <v>1209</v>
       </c>
@@ -12689,6 +13025,9 @@
       <c r="B432" t="s">
         <v>6</v>
       </c>
+      <c r="C432" t="s">
+        <v>1578</v>
+      </c>
       <c r="D432" t="s">
         <v>1210</v>
       </c>
@@ -12703,6 +13042,9 @@
       <c r="B433" t="s">
         <v>6</v>
       </c>
+      <c r="C433" t="s">
+        <v>1578</v>
+      </c>
       <c r="D433" t="s">
         <v>1211</v>
       </c>
@@ -12717,6 +13059,9 @@
       <c r="B434" t="s">
         <v>6</v>
       </c>
+      <c r="C434" t="s">
+        <v>1578</v>
+      </c>
       <c r="D434" t="s">
         <v>1212</v>
       </c>
@@ -12731,6 +13076,9 @@
       <c r="B435" t="s">
         <v>6</v>
       </c>
+      <c r="C435" t="s">
+        <v>1578</v>
+      </c>
       <c r="D435" t="s">
         <v>1213</v>
       </c>
@@ -12745,6 +13093,9 @@
       <c r="B436" t="s">
         <v>6</v>
       </c>
+      <c r="C436" t="s">
+        <v>1578</v>
+      </c>
       <c r="D436" t="s">
         <v>1214</v>
       </c>
@@ -12759,6 +13110,9 @@
       <c r="B437" t="s">
         <v>6</v>
       </c>
+      <c r="C437" t="s">
+        <v>1578</v>
+      </c>
       <c r="D437" t="s">
         <v>1215</v>
       </c>
@@ -12773,6 +13127,9 @@
       <c r="B438" t="s">
         <v>6</v>
       </c>
+      <c r="C438" t="s">
+        <v>1579</v>
+      </c>
       <c r="D438" t="s">
         <v>1216</v>
       </c>
@@ -12787,6 +13144,9 @@
       <c r="B439" t="s">
         <v>6</v>
       </c>
+      <c r="C439" t="s">
+        <v>1579</v>
+      </c>
       <c r="D439" t="s">
         <v>1217</v>
       </c>
@@ -12801,6 +13161,9 @@
       <c r="B440" t="s">
         <v>6</v>
       </c>
+      <c r="C440" t="s">
+        <v>1579</v>
+      </c>
       <c r="D440" t="s">
         <v>1218</v>
       </c>
@@ -12815,6 +13178,9 @@
       <c r="B441" t="s">
         <v>6</v>
       </c>
+      <c r="C441" t="s">
+        <v>1579</v>
+      </c>
       <c r="D441" t="s">
         <v>1219</v>
       </c>
@@ -12829,6 +13195,9 @@
       <c r="B442" t="s">
         <v>6</v>
       </c>
+      <c r="C442" t="s">
+        <v>1579</v>
+      </c>
       <c r="D442" t="s">
         <v>1220</v>
       </c>
@@ -12843,6 +13212,9 @@
       <c r="B443" t="s">
         <v>6</v>
       </c>
+      <c r="C443" t="s">
+        <v>1579</v>
+      </c>
       <c r="D443" t="s">
         <v>1221</v>
       </c>
@@ -12857,6 +13229,9 @@
       <c r="B444" t="s">
         <v>6</v>
       </c>
+      <c r="C444" t="s">
+        <v>1579</v>
+      </c>
       <c r="D444" t="s">
         <v>1222</v>
       </c>
@@ -12871,6 +13246,9 @@
       <c r="B445" t="s">
         <v>6</v>
       </c>
+      <c r="C445" t="s">
+        <v>1580</v>
+      </c>
       <c r="D445" t="s">
         <v>1223</v>
       </c>
@@ -12885,6 +13263,9 @@
       <c r="B446" t="s">
         <v>6</v>
       </c>
+      <c r="C446" t="s">
+        <v>1580</v>
+      </c>
       <c r="D446" t="s">
         <v>1224</v>
       </c>
@@ -12899,6 +13280,9 @@
       <c r="B447" t="s">
         <v>6</v>
       </c>
+      <c r="C447" t="s">
+        <v>1580</v>
+      </c>
       <c r="D447" t="s">
         <v>1225</v>
       </c>
@@ -12913,6 +13297,9 @@
       <c r="B448" t="s">
         <v>6</v>
       </c>
+      <c r="C448" t="s">
+        <v>1580</v>
+      </c>
       <c r="D448" t="s">
         <v>1226</v>
       </c>
@@ -12927,6 +13314,9 @@
       <c r="B449" t="s">
         <v>6</v>
       </c>
+      <c r="C449" t="s">
+        <v>1580</v>
+      </c>
       <c r="D449" t="s">
         <v>1227</v>
       </c>
@@ -12941,6 +13331,9 @@
       <c r="B450" t="s">
         <v>6</v>
       </c>
+      <c r="C450" t="s">
+        <v>1580</v>
+      </c>
       <c r="D450" t="s">
         <v>1228</v>
       </c>
@@ -12955,6 +13348,9 @@
       <c r="B451" t="s">
         <v>6</v>
       </c>
+      <c r="C451" t="s">
+        <v>1580</v>
+      </c>
       <c r="D451" t="s">
         <v>1229</v>
       </c>
@@ -12969,6 +13365,9 @@
       <c r="B452" t="s">
         <v>6</v>
       </c>
+      <c r="C452" t="s">
+        <v>1581</v>
+      </c>
       <c r="D452" t="s">
         <v>1230</v>
       </c>
@@ -12983,6 +13382,9 @@
       <c r="B453" t="s">
         <v>6</v>
       </c>
+      <c r="C453" t="s">
+        <v>1581</v>
+      </c>
       <c r="D453" t="s">
         <v>1231</v>
       </c>
@@ -12997,6 +13399,9 @@
       <c r="B454" t="s">
         <v>6</v>
       </c>
+      <c r="C454" t="s">
+        <v>1581</v>
+      </c>
       <c r="D454" t="s">
         <v>1232</v>
       </c>
@@ -13011,6 +13416,9 @@
       <c r="B455" t="s">
         <v>6</v>
       </c>
+      <c r="C455" t="s">
+        <v>1581</v>
+      </c>
       <c r="D455" t="s">
         <v>1233</v>
       </c>
@@ -13025,6 +13433,9 @@
       <c r="B456" t="s">
         <v>6</v>
       </c>
+      <c r="C456" t="s">
+        <v>1581</v>
+      </c>
       <c r="D456" t="s">
         <v>1234</v>
       </c>
@@ -13039,6 +13450,9 @@
       <c r="B457" t="s">
         <v>6</v>
       </c>
+      <c r="C457" t="s">
+        <v>1581</v>
+      </c>
       <c r="D457" t="s">
         <v>1235</v>
       </c>
@@ -13053,6 +13467,9 @@
       <c r="B458" t="s">
         <v>6</v>
       </c>
+      <c r="C458" t="s">
+        <v>1581</v>
+      </c>
       <c r="D458" t="s">
         <v>1236</v>
       </c>
@@ -13067,6 +13484,9 @@
       <c r="B459" t="s">
         <v>6</v>
       </c>
+      <c r="C459" t="s">
+        <v>1582</v>
+      </c>
       <c r="D459" t="s">
         <v>1237</v>
       </c>
@@ -13081,6 +13501,9 @@
       <c r="B460" t="s">
         <v>6</v>
       </c>
+      <c r="C460" t="s">
+        <v>1582</v>
+      </c>
       <c r="D460" t="s">
         <v>1238</v>
       </c>
@@ -13095,6 +13518,9 @@
       <c r="B461" t="s">
         <v>6</v>
       </c>
+      <c r="C461" t="s">
+        <v>1582</v>
+      </c>
       <c r="D461" t="s">
         <v>1239</v>
       </c>
@@ -13109,6 +13535,9 @@
       <c r="B462" t="s">
         <v>6</v>
       </c>
+      <c r="C462" t="s">
+        <v>1582</v>
+      </c>
       <c r="D462" t="s">
         <v>1240</v>
       </c>
@@ -13123,6 +13552,9 @@
       <c r="B463" t="s">
         <v>6</v>
       </c>
+      <c r="C463" t="s">
+        <v>1582</v>
+      </c>
       <c r="D463" t="s">
         <v>1241</v>
       </c>
@@ -13137,6 +13569,9 @@
       <c r="B464" t="s">
         <v>6</v>
       </c>
+      <c r="C464" t="s">
+        <v>1582</v>
+      </c>
       <c r="D464" t="s">
         <v>1242</v>
       </c>
@@ -13151,6 +13586,9 @@
       <c r="B465" t="s">
         <v>6</v>
       </c>
+      <c r="C465" t="s">
+        <v>1583</v>
+      </c>
       <c r="D465" t="s">
         <v>1243</v>
       </c>
@@ -13165,6 +13603,9 @@
       <c r="B466" t="s">
         <v>6</v>
       </c>
+      <c r="C466" t="s">
+        <v>1583</v>
+      </c>
       <c r="D466" t="s">
         <v>1244</v>
       </c>
@@ -13179,6 +13620,9 @@
       <c r="B467" t="s">
         <v>6</v>
       </c>
+      <c r="C467" t="s">
+        <v>1583</v>
+      </c>
       <c r="D467" t="s">
         <v>1245</v>
       </c>
@@ -13193,6 +13637,9 @@
       <c r="B468" t="s">
         <v>6</v>
       </c>
+      <c r="C468" t="s">
+        <v>1583</v>
+      </c>
       <c r="D468" t="s">
         <v>1246</v>
       </c>
@@ -13207,6 +13654,9 @@
       <c r="B469" t="s">
         <v>6</v>
       </c>
+      <c r="C469" t="s">
+        <v>1583</v>
+      </c>
       <c r="D469" t="s">
         <v>1247</v>
       </c>
@@ -13221,6 +13671,9 @@
       <c r="B470" t="s">
         <v>6</v>
       </c>
+      <c r="C470" t="s">
+        <v>1583</v>
+      </c>
       <c r="D470" t="s">
         <v>1248</v>
       </c>
@@ -13235,6 +13688,9 @@
       <c r="B471" t="s">
         <v>6</v>
       </c>
+      <c r="C471" t="s">
+        <v>1584</v>
+      </c>
       <c r="D471" t="s">
         <v>1249</v>
       </c>
@@ -13249,6 +13705,9 @@
       <c r="B472" t="s">
         <v>6</v>
       </c>
+      <c r="C472" t="s">
+        <v>1584</v>
+      </c>
       <c r="D472" t="s">
         <v>1250</v>
       </c>
@@ -13263,6 +13722,9 @@
       <c r="B473" t="s">
         <v>6</v>
       </c>
+      <c r="C473" t="s">
+        <v>1584</v>
+      </c>
       <c r="D473" t="s">
         <v>1251</v>
       </c>
@@ -13277,6 +13739,9 @@
       <c r="B474" t="s">
         <v>6</v>
       </c>
+      <c r="C474" t="s">
+        <v>1584</v>
+      </c>
       <c r="D474" t="s">
         <v>1252</v>
       </c>
@@ -13291,6 +13756,9 @@
       <c r="B475" t="s">
         <v>6</v>
       </c>
+      <c r="C475" t="s">
+        <v>1584</v>
+      </c>
       <c r="D475" t="s">
         <v>1253</v>
       </c>
@@ -13305,6 +13773,9 @@
       <c r="B476" t="s">
         <v>6</v>
       </c>
+      <c r="C476" t="s">
+        <v>1584</v>
+      </c>
       <c r="D476" t="s">
         <v>1254</v>
       </c>
@@ -13319,6 +13790,9 @@
       <c r="B477" t="s">
         <v>6</v>
       </c>
+      <c r="C477" t="s">
+        <v>1585</v>
+      </c>
       <c r="D477" t="s">
         <v>1255</v>
       </c>
@@ -13333,6 +13807,9 @@
       <c r="B478" t="s">
         <v>6</v>
       </c>
+      <c r="C478" t="s">
+        <v>1585</v>
+      </c>
       <c r="D478" t="s">
         <v>1256</v>
       </c>
@@ -13347,6 +13824,9 @@
       <c r="B479" t="s">
         <v>6</v>
       </c>
+      <c r="C479" t="s">
+        <v>1585</v>
+      </c>
       <c r="D479" t="s">
         <v>1257</v>
       </c>
@@ -13361,6 +13841,9 @@
       <c r="B480" t="s">
         <v>6</v>
       </c>
+      <c r="C480" t="s">
+        <v>1585</v>
+      </c>
       <c r="D480" t="s">
         <v>1258</v>
       </c>
@@ -13375,6 +13858,9 @@
       <c r="B481" t="s">
         <v>6</v>
       </c>
+      <c r="C481" t="s">
+        <v>1585</v>
+      </c>
       <c r="D481" t="s">
         <v>1259</v>
       </c>
@@ -13389,6 +13875,9 @@
       <c r="B482" t="s">
         <v>6</v>
       </c>
+      <c r="C482" t="s">
+        <v>1585</v>
+      </c>
       <c r="D482" t="s">
         <v>1260</v>
       </c>
@@ -13403,6 +13892,9 @@
       <c r="B483" t="s">
         <v>6</v>
       </c>
+      <c r="C483" t="s">
+        <v>1586</v>
+      </c>
       <c r="D483" t="s">
         <v>1261</v>
       </c>
@@ -13417,6 +13909,9 @@
       <c r="B484" t="s">
         <v>6</v>
       </c>
+      <c r="C484" t="s">
+        <v>1586</v>
+      </c>
       <c r="D484" t="s">
         <v>1262</v>
       </c>
@@ -13431,6 +13926,9 @@
       <c r="B485" t="s">
         <v>6</v>
       </c>
+      <c r="C485" t="s">
+        <v>1586</v>
+      </c>
       <c r="D485" t="s">
         <v>1263</v>
       </c>
@@ -13445,6 +13943,9 @@
       <c r="B486" t="s">
         <v>6</v>
       </c>
+      <c r="C486" t="s">
+        <v>1586</v>
+      </c>
       <c r="D486" t="s">
         <v>1264</v>
       </c>
@@ -13459,6 +13960,9 @@
       <c r="B487" t="s">
         <v>6</v>
       </c>
+      <c r="C487" t="s">
+        <v>1586</v>
+      </c>
       <c r="D487" t="s">
         <v>1265</v>
       </c>
@@ -13473,6 +13977,9 @@
       <c r="B488" t="s">
         <v>6</v>
       </c>
+      <c r="C488" t="s">
+        <v>1586</v>
+      </c>
       <c r="D488" t="s">
         <v>1266</v>
       </c>
@@ -13487,6 +13994,9 @@
       <c r="B489" t="s">
         <v>6</v>
       </c>
+      <c r="C489" t="s">
+        <v>1587</v>
+      </c>
       <c r="D489" t="s">
         <v>1267</v>
       </c>
@@ -13501,6 +14011,9 @@
       <c r="B490" t="s">
         <v>6</v>
       </c>
+      <c r="C490" t="s">
+        <v>1587</v>
+      </c>
       <c r="D490" t="s">
         <v>1268</v>
       </c>
@@ -13515,6 +14028,9 @@
       <c r="B491" t="s">
         <v>6</v>
       </c>
+      <c r="C491" t="s">
+        <v>1587</v>
+      </c>
       <c r="D491" t="s">
         <v>1269</v>
       </c>
@@ -13529,6 +14045,9 @@
       <c r="B492" t="s">
         <v>6</v>
       </c>
+      <c r="C492" t="s">
+        <v>1587</v>
+      </c>
       <c r="D492" t="s">
         <v>1270</v>
       </c>
@@ -13543,6 +14062,9 @@
       <c r="B493" t="s">
         <v>6</v>
       </c>
+      <c r="C493" t="s">
+        <v>1587</v>
+      </c>
       <c r="D493" t="s">
         <v>1271</v>
       </c>
@@ -13557,6 +14079,9 @@
       <c r="B494" t="s">
         <v>6</v>
       </c>
+      <c r="C494" t="s">
+        <v>1587</v>
+      </c>
       <c r="D494" t="s">
         <v>1272</v>
       </c>
@@ -13571,6 +14096,9 @@
       <c r="B495" t="s">
         <v>6</v>
       </c>
+      <c r="C495" t="s">
+        <v>1587</v>
+      </c>
       <c r="D495" t="s">
         <v>1273</v>
       </c>
@@ -13585,6 +14113,9 @@
       <c r="B496" t="s">
         <v>6</v>
       </c>
+      <c r="C496" t="s">
+        <v>1588</v>
+      </c>
       <c r="D496" t="s">
         <v>1274</v>
       </c>
@@ -13599,6 +14130,9 @@
       <c r="B497" t="s">
         <v>6</v>
       </c>
+      <c r="C497" t="s">
+        <v>1588</v>
+      </c>
       <c r="D497" t="s">
         <v>1275</v>
       </c>
@@ -13613,6 +14147,9 @@
       <c r="B498" t="s">
         <v>6</v>
       </c>
+      <c r="C498" t="s">
+        <v>1588</v>
+      </c>
       <c r="D498" t="s">
         <v>1276</v>
       </c>
@@ -13627,6 +14164,9 @@
       <c r="B499" t="s">
         <v>6</v>
       </c>
+      <c r="C499" t="s">
+        <v>1588</v>
+      </c>
       <c r="D499" t="s">
         <v>1277</v>
       </c>
@@ -13641,6 +14181,9 @@
       <c r="B500" t="s">
         <v>6</v>
       </c>
+      <c r="C500" t="s">
+        <v>1588</v>
+      </c>
       <c r="D500" t="s">
         <v>1278</v>
       </c>
@@ -13655,6 +14198,9 @@
       <c r="B501" t="s">
         <v>6</v>
       </c>
+      <c r="C501" t="s">
+        <v>1588</v>
+      </c>
       <c r="D501" t="s">
         <v>1279</v>
       </c>
@@ -13669,6 +14215,9 @@
       <c r="B502" t="s">
         <v>6</v>
       </c>
+      <c r="C502" t="s">
+        <v>1589</v>
+      </c>
       <c r="D502" t="s">
         <v>1280</v>
       </c>
@@ -13683,6 +14232,9 @@
       <c r="B503" t="s">
         <v>6</v>
       </c>
+      <c r="C503" t="s">
+        <v>1589</v>
+      </c>
       <c r="D503" t="s">
         <v>1281</v>
       </c>
@@ -13697,6 +14249,9 @@
       <c r="B504" t="s">
         <v>6</v>
       </c>
+      <c r="C504" t="s">
+        <v>1589</v>
+      </c>
       <c r="D504" t="s">
         <v>1282</v>
       </c>
@@ -13711,6 +14266,9 @@
       <c r="B505" t="s">
         <v>6</v>
       </c>
+      <c r="C505" t="s">
+        <v>1589</v>
+      </c>
       <c r="D505" t="s">
         <v>1283</v>
       </c>
@@ -13725,6 +14283,9 @@
       <c r="B506" t="s">
         <v>6</v>
       </c>
+      <c r="C506" t="s">
+        <v>1589</v>
+      </c>
       <c r="D506" t="s">
         <v>1284</v>
       </c>
@@ -13739,6 +14300,9 @@
       <c r="B507" t="s">
         <v>6</v>
       </c>
+      <c r="C507" t="s">
+        <v>1589</v>
+      </c>
       <c r="D507" t="s">
         <v>1285</v>
       </c>
@@ -13753,6 +14317,9 @@
       <c r="B508" t="s">
         <v>6</v>
       </c>
+      <c r="C508" t="s">
+        <v>1590</v>
+      </c>
       <c r="D508" t="s">
         <v>1286</v>
       </c>
@@ -13767,6 +14334,9 @@
       <c r="B509" t="s">
         <v>6</v>
       </c>
+      <c r="C509" t="s">
+        <v>1590</v>
+      </c>
       <c r="D509" t="s">
         <v>1287</v>
       </c>
@@ -13781,6 +14351,9 @@
       <c r="B510" t="s">
         <v>6</v>
       </c>
+      <c r="C510" t="s">
+        <v>1590</v>
+      </c>
       <c r="D510" t="s">
         <v>1288</v>
       </c>
@@ -13795,6 +14368,9 @@
       <c r="B511" t="s">
         <v>6</v>
       </c>
+      <c r="C511" t="s">
+        <v>1590</v>
+      </c>
       <c r="D511" t="s">
         <v>1289</v>
       </c>
@@ -13809,6 +14385,9 @@
       <c r="B512" t="s">
         <v>6</v>
       </c>
+      <c r="C512" t="s">
+        <v>1590</v>
+      </c>
       <c r="D512" t="s">
         <v>1290</v>
       </c>
@@ -13823,6 +14402,9 @@
       <c r="B513" t="s">
         <v>6</v>
       </c>
+      <c r="C513" t="s">
+        <v>1590</v>
+      </c>
       <c r="D513" t="s">
         <v>1291</v>
       </c>
@@ -13837,6 +14419,9 @@
       <c r="B514" t="s">
         <v>6</v>
       </c>
+      <c r="C514" t="s">
+        <v>1591</v>
+      </c>
       <c r="D514" t="s">
         <v>1292</v>
       </c>
@@ -13851,6 +14436,9 @@
       <c r="B515" t="s">
         <v>6</v>
       </c>
+      <c r="C515" t="s">
+        <v>1591</v>
+      </c>
       <c r="D515" t="s">
         <v>1293</v>
       </c>
@@ -13865,6 +14453,9 @@
       <c r="B516" t="s">
         <v>6</v>
       </c>
+      <c r="C516" t="s">
+        <v>1591</v>
+      </c>
       <c r="D516" t="s">
         <v>1294</v>
       </c>
@@ -13879,6 +14470,9 @@
       <c r="B517" t="s">
         <v>6</v>
       </c>
+      <c r="C517" t="s">
+        <v>1591</v>
+      </c>
       <c r="D517" t="s">
         <v>1295</v>
       </c>
@@ -13893,6 +14487,9 @@
       <c r="B518" t="s">
         <v>6</v>
       </c>
+      <c r="C518" t="s">
+        <v>1591</v>
+      </c>
       <c r="D518" t="s">
         <v>1296</v>
       </c>
@@ -13907,6 +14504,9 @@
       <c r="B519" t="s">
         <v>6</v>
       </c>
+      <c r="C519" t="s">
+        <v>1591</v>
+      </c>
       <c r="D519" t="s">
         <v>1297</v>
       </c>
@@ -13921,6 +14521,9 @@
       <c r="B520" t="s">
         <v>6</v>
       </c>
+      <c r="C520" t="s">
+        <v>1591</v>
+      </c>
       <c r="D520" t="s">
         <v>1298</v>
       </c>
@@ -13935,6 +14538,9 @@
       <c r="B521" t="s">
         <v>6</v>
       </c>
+      <c r="C521" t="s">
+        <v>1592</v>
+      </c>
       <c r="D521" t="s">
         <v>1299</v>
       </c>
@@ -13949,6 +14555,9 @@
       <c r="B522" t="s">
         <v>6</v>
       </c>
+      <c r="C522" t="s">
+        <v>1592</v>
+      </c>
       <c r="D522" t="s">
         <v>1300</v>
       </c>
@@ -13963,6 +14572,9 @@
       <c r="B523" t="s">
         <v>6</v>
       </c>
+      <c r="C523" t="s">
+        <v>1592</v>
+      </c>
       <c r="D523" t="s">
         <v>1301</v>
       </c>
@@ -13977,6 +14589,9 @@
       <c r="B524" t="s">
         <v>6</v>
       </c>
+      <c r="C524" t="s">
+        <v>1592</v>
+      </c>
       <c r="D524" t="s">
         <v>1302</v>
       </c>
@@ -13991,6 +14606,9 @@
       <c r="B525" t="s">
         <v>6</v>
       </c>
+      <c r="C525" t="s">
+        <v>1592</v>
+      </c>
       <c r="D525" t="s">
         <v>1303</v>
       </c>
@@ -14005,6 +14623,9 @@
       <c r="B526" t="s">
         <v>6</v>
       </c>
+      <c r="C526" t="s">
+        <v>1592</v>
+      </c>
       <c r="D526" t="s">
         <v>1304</v>
       </c>
@@ -14019,6 +14640,9 @@
       <c r="B527" t="s">
         <v>6</v>
       </c>
+      <c r="C527" t="s">
+        <v>1593</v>
+      </c>
       <c r="D527" t="s">
         <v>1305</v>
       </c>
@@ -14033,6 +14657,9 @@
       <c r="B528" t="s">
         <v>6</v>
       </c>
+      <c r="C528" t="s">
+        <v>1593</v>
+      </c>
       <c r="D528" t="s">
         <v>1306</v>
       </c>
@@ -14047,6 +14674,9 @@
       <c r="B529" t="s">
         <v>6</v>
       </c>
+      <c r="C529" t="s">
+        <v>1593</v>
+      </c>
       <c r="D529" t="s">
         <v>1307</v>
       </c>
@@ -14061,6 +14691,9 @@
       <c r="B530" t="s">
         <v>6</v>
       </c>
+      <c r="C530" t="s">
+        <v>1593</v>
+      </c>
       <c r="D530" t="s">
         <v>1308</v>
       </c>
@@ -14075,6 +14708,9 @@
       <c r="B531" t="s">
         <v>6</v>
       </c>
+      <c r="C531" t="s">
+        <v>1593</v>
+      </c>
       <c r="D531" t="s">
         <v>1309</v>
       </c>
@@ -14089,6 +14725,9 @@
       <c r="B532" t="s">
         <v>6</v>
       </c>
+      <c r="C532" t="s">
+        <v>1593</v>
+      </c>
       <c r="D532" t="s">
         <v>1310</v>
       </c>
@@ -14103,6 +14742,9 @@
       <c r="B533" t="s">
         <v>6</v>
       </c>
+      <c r="C533" t="s">
+        <v>1594</v>
+      </c>
       <c r="D533" t="s">
         <v>1311</v>
       </c>
@@ -14117,6 +14759,9 @@
       <c r="B534" t="s">
         <v>6</v>
       </c>
+      <c r="C534" t="s">
+        <v>1594</v>
+      </c>
       <c r="D534" t="s">
         <v>1312</v>
       </c>
@@ -14131,6 +14776,9 @@
       <c r="B535" t="s">
         <v>6</v>
       </c>
+      <c r="C535" t="s">
+        <v>1594</v>
+      </c>
       <c r="D535" t="s">
         <v>1313</v>
       </c>
@@ -14145,6 +14793,9 @@
       <c r="B536" t="s">
         <v>6</v>
       </c>
+      <c r="C536" t="s">
+        <v>1594</v>
+      </c>
       <c r="D536" t="s">
         <v>1314</v>
       </c>
@@ -14159,6 +14810,9 @@
       <c r="B537" t="s">
         <v>6</v>
       </c>
+      <c r="C537" t="s">
+        <v>1594</v>
+      </c>
       <c r="D537" t="s">
         <v>1315</v>
       </c>
@@ -14173,6 +14827,9 @@
       <c r="B538" t="s">
         <v>6</v>
       </c>
+      <c r="C538" t="s">
+        <v>1595</v>
+      </c>
       <c r="D538" t="s">
         <v>1316</v>
       </c>
@@ -14187,6 +14844,9 @@
       <c r="B539" t="s">
         <v>6</v>
       </c>
+      <c r="C539" t="s">
+        <v>1595</v>
+      </c>
       <c r="D539" t="s">
         <v>1317</v>
       </c>
@@ -14201,6 +14861,9 @@
       <c r="B540" t="s">
         <v>6</v>
       </c>
+      <c r="C540" t="s">
+        <v>1595</v>
+      </c>
       <c r="D540" t="s">
         <v>1318</v>
       </c>
@@ -14215,6 +14878,9 @@
       <c r="B541" t="s">
         <v>6</v>
       </c>
+      <c r="C541" t="s">
+        <v>1595</v>
+      </c>
       <c r="D541" t="s">
         <v>1319</v>
       </c>
@@ -14229,6 +14895,9 @@
       <c r="B542" t="s">
         <v>6</v>
       </c>
+      <c r="C542" t="s">
+        <v>1595</v>
+      </c>
       <c r="D542" t="s">
         <v>1320</v>
       </c>
@@ -14243,6 +14912,9 @@
       <c r="B543" t="s">
         <v>6</v>
       </c>
+      <c r="C543" t="s">
+        <v>1595</v>
+      </c>
       <c r="D543" t="s">
         <v>1321</v>
       </c>
@@ -14257,6 +14929,9 @@
       <c r="B544" t="s">
         <v>6</v>
       </c>
+      <c r="C544" t="s">
+        <v>1595</v>
+      </c>
       <c r="D544" t="s">
         <v>1322</v>
       </c>
@@ -14271,6 +14946,9 @@
       <c r="B545" t="s">
         <v>6</v>
       </c>
+      <c r="C545" t="s">
+        <v>1596</v>
+      </c>
       <c r="D545" t="s">
         <v>1323</v>
       </c>
@@ -14285,6 +14963,9 @@
       <c r="B546" t="s">
         <v>6</v>
       </c>
+      <c r="C546" t="s">
+        <v>1596</v>
+      </c>
       <c r="D546" t="s">
         <v>1324</v>
       </c>
@@ -14299,6 +14980,9 @@
       <c r="B547" t="s">
         <v>6</v>
       </c>
+      <c r="C547" t="s">
+        <v>1596</v>
+      </c>
       <c r="D547" t="s">
         <v>1325</v>
       </c>
@@ -14313,6 +14997,9 @@
       <c r="B548" t="s">
         <v>6</v>
       </c>
+      <c r="C548" t="s">
+        <v>1596</v>
+      </c>
       <c r="D548" t="s">
         <v>1326</v>
       </c>
@@ -14327,6 +15014,9 @@
       <c r="B549" t="s">
         <v>6</v>
       </c>
+      <c r="C549" t="s">
+        <v>1596</v>
+      </c>
       <c r="D549" t="s">
         <v>1327</v>
       </c>
@@ -14340,6 +15030,9 @@
       </c>
       <c r="B550" t="s">
         <v>6</v>
+      </c>
+      <c r="C550" t="s">
+        <v>1596</v>
       </c>
       <c r="D550" t="s">
         <v>1328</v>

</xml_diff>